<commit_message>
Flux specific variables corrected
</commit_message>
<xml_diff>
--- a/specific_variables/flux-estimates-level1.xlsx
+++ b/specific_variables/flux-estimates-level1.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10308"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10413"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/heather/Desktop/NC_parse_master/specific_variables/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/heather/Desktop/ace-ceda-master/specific_variables/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{45112136-0E3C-B949-B728-17688AE04084}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C8547DAA-986C-CA4E-BA3C-06A03DB35638}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="50040" yWindow="-3140" windowWidth="16360" windowHeight="21140" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="327" uniqueCount="82">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="351" uniqueCount="86">
   <si>
     <t>Variable</t>
   </si>
@@ -109,9 +109,6 @@
     <t>J m-2 s-1</t>
   </si>
   <si>
-    <t>Buoyancy Flux (rho.cp.&lt;w'Ts'&gt;)</t>
-  </si>
-  <si>
     <t>cell_methods</t>
   </si>
   <si>
@@ -247,12 +244,6 @@
     <t>bad_data, good_data, suspect_data</t>
   </si>
   <si>
-    <t>0,1, 2, 3</t>
-  </si>
-  <si>
-    <t>bad_data, good_data _good_for_reasearch, suspect_data_good_for_general_use, suspect_data_requires_further_checking_but_may_be_ok_for_general_use</t>
-  </si>
-  <si>
     <t>qc_flag_kurtosis_u</t>
   </si>
   <si>
@@ -266,13 +257,39 @@
   </si>
   <si>
     <t>Height of instrument platform above snow surface</t>
+  </si>
+  <si>
+    <t>&lt;derived from file&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Buoyancy Flux (&lt;w'Ts'&gt;) </t>
+  </si>
+  <si>
+    <t>0b,1b, 2b</t>
+  </si>
+  <si>
+    <t>bad_data
+good_data 
+suspect_data</t>
+  </si>
+  <si>
+    <t>0b,1b, 2b, 3b</t>
+  </si>
+  <si>
+    <t>bad_data
+good_data _good_for_reasearch
+suspect_data_good_for_general_use
+suspect_data_requires_further_checking_but_may_be_ok_for_general_use</t>
+  </si>
+  <si>
+    <t>time: mean</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -307,6 +324,12 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -335,7 +358,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -347,9 +370,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -368,19 +388,9 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -388,6 +398,13 @@
     </xf>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -706,10 +723,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:F971"/>
+  <dimension ref="A1:F968"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A24" workbookViewId="0">
-      <selection activeCell="A44" sqref="A44"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A41" sqref="A41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -744,387 +761,440 @@
       </c>
     </row>
     <row r="2" spans="1:6" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A2" t="s">
+      <c r="A2" s="12" t="s">
         <v>7</v>
       </c>
-      <c r="C2" s="4"/>
+      <c r="B2" s="12"/>
+      <c r="C2" s="5"/>
     </row>
     <row r="3" spans="1:6" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B3" t="s">
+      <c r="A3" s="12"/>
+      <c r="B3" s="12" t="s">
         <v>8</v>
       </c>
-      <c r="C3" s="6" t="s">
+      <c r="C3" s="5" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="4" spans="1:6" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B4" t="s">
+      <c r="A4" s="12"/>
+      <c r="B4" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="C4" s="4" t="s">
+      <c r="C4" s="5" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="5" spans="1:6" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B5" t="s">
+      <c r="A5" s="12"/>
+      <c r="B5" s="12" t="s">
         <v>3</v>
       </c>
-      <c r="C5" s="6" t="s">
+      <c r="C5" s="5" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="6" spans="1:6" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B6" t="s">
-        <v>13</v>
-      </c>
-      <c r="C6" s="4"/>
+      <c r="A6" s="12"/>
+      <c r="B6" s="12" t="s">
+        <v>14</v>
+      </c>
+      <c r="C6" s="5" t="s">
+        <v>15</v>
+      </c>
       <c r="D6" s="4"/>
     </row>
     <row r="7" spans="1:6" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B7" t="s">
+      <c r="A7" s="12"/>
+      <c r="B7" s="12" t="s">
+        <v>16</v>
+      </c>
+      <c r="C7" s="15">
+        <v>-1E+20</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" ht="12" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A8" s="12"/>
+      <c r="B8" s="12" t="s">
+        <v>17</v>
+      </c>
+      <c r="C8" s="14" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" ht="12" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A9" s="12"/>
+      <c r="B9" s="12" t="s">
+        <v>18</v>
+      </c>
+      <c r="C9" s="14" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" ht="12" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A10" s="12"/>
+      <c r="B10" s="12" t="s">
+        <v>19</v>
+      </c>
+      <c r="C10" s="5" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" ht="12" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A11" s="12"/>
+      <c r="B11" s="12"/>
+      <c r="C11" s="5"/>
+    </row>
+    <row r="12" spans="1:6" ht="12" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A12" s="12" t="s">
+        <v>21</v>
+      </c>
+      <c r="B12" s="12"/>
+      <c r="C12" s="5"/>
+    </row>
+    <row r="13" spans="1:6" ht="12" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A13" s="12"/>
+      <c r="B13" s="12" t="s">
+        <v>8</v>
+      </c>
+      <c r="C13" s="5" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" ht="12" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A14" s="12"/>
+      <c r="B14" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="C14" s="5" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" ht="12" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A15" s="12"/>
+      <c r="B15" s="12" t="s">
+        <v>3</v>
+      </c>
+      <c r="C15" s="14" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" ht="12" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A16" s="12"/>
+      <c r="B16" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="C7" s="6" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B8" t="s">
+      <c r="C16" s="5" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" ht="12" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A17" s="12"/>
+      <c r="B17" s="12" t="s">
         <v>16</v>
       </c>
-      <c r="C8" s="7">
+      <c r="C17" s="15">
         <v>-1E+20</v>
       </c>
-    </row>
-    <row r="9" spans="1:6" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B9" t="s">
+      <c r="D17" s="4"/>
+    </row>
+    <row r="18" spans="1:4" ht="12" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A18" s="12"/>
+      <c r="B18" s="12" t="s">
+        <v>17</v>
+      </c>
+      <c r="C18" s="7" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" ht="12" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A19" s="12"/>
+      <c r="B19" s="12" t="s">
+        <v>18</v>
+      </c>
+      <c r="C19" s="7" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" ht="12" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A20" s="12"/>
+      <c r="B20" s="12" t="s">
         <v>19</v>
       </c>
-      <c r="C9" s="4" t="s">
+      <c r="C20" s="5" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="10" spans="1:6" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="C10" s="4"/>
-    </row>
-    <row r="11" spans="1:6" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A11" t="s">
-        <v>21</v>
-      </c>
-      <c r="C11" s="4"/>
-    </row>
-    <row r="12" spans="1:6" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B12" t="s">
+    <row r="21" spans="1:4" ht="12" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A21" s="12"/>
+      <c r="B21" s="12"/>
+      <c r="C21" s="12"/>
+    </row>
+    <row r="22" spans="1:4" ht="12" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A22" s="12" t="s">
+        <v>76</v>
+      </c>
+      <c r="B22" s="12"/>
+      <c r="C22" s="12"/>
+    </row>
+    <row r="23" spans="1:4" ht="12" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A23" s="12"/>
+      <c r="B23" s="12" t="s">
         <v>8</v>
       </c>
-      <c r="C12" s="6" t="s">
+      <c r="C23" s="13" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="13" spans="1:6" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B13" t="s">
+    <row r="24" spans="1:4" ht="12" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A24" s="12"/>
+      <c r="B24" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="C13" s="4" t="s">
+      <c r="C24" s="12" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="14" spans="1:6" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B14" t="s">
+    <row r="25" spans="1:4" ht="12" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A25" s="12"/>
+      <c r="B25" s="12" t="s">
         <v>3</v>
       </c>
-      <c r="C14" s="5" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B15" t="s">
-        <v>13</v>
-      </c>
-      <c r="C15" s="4"/>
-    </row>
-    <row r="16" spans="1:6" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B16" t="s">
+      <c r="C25" s="14" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" ht="12" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A26" s="12"/>
+      <c r="B26" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="C16" s="4" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B17" t="s">
+      <c r="C26" s="12" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" ht="12" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A27" s="12"/>
+      <c r="B27" s="12" t="s">
         <v>16</v>
       </c>
-      <c r="C17" s="7">
+      <c r="C27" s="15">
         <v>-1E+20</v>
       </c>
-      <c r="D17" s="4"/>
-    </row>
-    <row r="18" spans="1:4" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B18" t="s">
+    </row>
+    <row r="28" spans="1:4" ht="12" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A28" s="12"/>
+      <c r="B28" s="12" t="s">
         <v>17</v>
       </c>
-      <c r="C18" s="8">
+      <c r="C28" s="7" t="s">
+        <v>79</v>
+      </c>
+      <c r="D28" s="4"/>
+    </row>
+    <row r="29" spans="1:4" ht="12" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A29" s="12"/>
+      <c r="B29" s="12" t="s">
+        <v>18</v>
+      </c>
+      <c r="C29" s="7" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" ht="12" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A30" s="12"/>
+      <c r="B30" s="12" t="s">
+        <v>29</v>
+      </c>
+      <c r="C30" s="18" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" ht="12" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A31" s="12"/>
+      <c r="B31" s="12" t="s">
+        <v>19</v>
+      </c>
+      <c r="C31" s="12" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" ht="12" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A32" s="12"/>
+      <c r="B32" s="12"/>
+      <c r="C32" s="5"/>
+    </row>
+    <row r="33" spans="1:4" ht="12" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A33" s="12" t="s">
+        <v>25</v>
+      </c>
+      <c r="B33" s="12"/>
+      <c r="C33" s="5"/>
+    </row>
+    <row r="34" spans="1:4" ht="12" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A34" s="12"/>
+      <c r="B34" s="12" t="s">
+        <v>8</v>
+      </c>
+      <c r="C34" s="5" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" ht="12" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A35" s="12"/>
+      <c r="B35" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="C35" s="5" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" ht="12" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A36" s="12"/>
+      <c r="B36" s="12" t="s">
+        <v>3</v>
+      </c>
+      <c r="C36" s="14">
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="1:4" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B19" t="s">
+    <row r="37" spans="1:4" ht="12" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A37" s="12"/>
+      <c r="B37" s="12" t="s">
+        <v>14</v>
+      </c>
+      <c r="C37" s="5" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" ht="12" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A38" s="12"/>
+      <c r="B38" s="12" t="s">
+        <v>16</v>
+      </c>
+      <c r="C38" s="15">
+        <v>-1E+20</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" ht="12" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A39" s="12"/>
+      <c r="B39" s="12" t="s">
+        <v>17</v>
+      </c>
+      <c r="C39" s="7" t="s">
+        <v>79</v>
+      </c>
+      <c r="D39" s="4"/>
+    </row>
+    <row r="40" spans="1:4" ht="12" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A40" s="12"/>
+      <c r="B40" s="12" t="s">
         <v>18</v>
       </c>
-      <c r="C19" s="8">
-        <v>3600</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B20" t="s">
+      <c r="C40" s="7" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" ht="12" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A41" s="12"/>
+      <c r="B41" s="12" t="s">
         <v>19</v>
       </c>
-      <c r="C20" s="4" t="s">
+      <c r="C41" s="5" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="21" spans="1:4" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A21" s="17"/>
-      <c r="B21" s="17"/>
-      <c r="C21" s="17"/>
-    </row>
-    <row r="22" spans="1:4" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A22" s="17" t="s">
+    <row r="42" spans="1:4" ht="12" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A42" s="12"/>
+      <c r="B42" s="12"/>
+      <c r="C42" s="5"/>
+    </row>
+    <row r="43" spans="1:4" ht="12" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A43" s="12" t="s">
+        <v>27</v>
+      </c>
+      <c r="B43" s="12"/>
+      <c r="C43" s="5"/>
+    </row>
+    <row r="44" spans="1:4" ht="12" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A44" s="12"/>
+      <c r="B44" s="12" t="s">
+        <v>8</v>
+      </c>
+      <c r="C44" s="5" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" ht="12" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A45" s="12"/>
+      <c r="B45" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="C45" s="5" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" ht="12" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A46" s="12"/>
+      <c r="B46" s="12" t="s">
+        <v>3</v>
+      </c>
+      <c r="C46" s="5" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4" ht="12" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A47" s="12"/>
+      <c r="B47" s="12" t="s">
+        <v>14</v>
+      </c>
+      <c r="C47" s="16" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4" ht="12" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A48" s="12"/>
+      <c r="B48" s="12" t="s">
+        <v>16</v>
+      </c>
+      <c r="C48" s="15">
+        <v>-1E+20</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4" ht="12" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A49" s="12"/>
+      <c r="B49" s="12" t="s">
+        <v>17</v>
+      </c>
+      <c r="C49" s="7" t="s">
         <v>79</v>
       </c>
-      <c r="B22" s="17"/>
-      <c r="C22" s="17"/>
-    </row>
-    <row r="23" spans="1:4" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A23" s="17"/>
-      <c r="B23" s="17" t="s">
-        <v>8</v>
-      </c>
-      <c r="C23" s="18" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A24" s="17"/>
-      <c r="B24" s="17" t="s">
-        <v>10</v>
-      </c>
-      <c r="C24" s="17" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="25" spans="1:4" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A25" s="17"/>
-      <c r="B25" s="17" t="s">
-        <v>3</v>
-      </c>
-      <c r="C25" s="19" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="26" spans="1:4" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A26" s="17"/>
-      <c r="B26" s="17" t="s">
-        <v>13</v>
-      </c>
-      <c r="C26" s="17"/>
-    </row>
-    <row r="27" spans="1:4" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A27" s="17"/>
-      <c r="B27" s="17" t="s">
-        <v>14</v>
-      </c>
-      <c r="C27" s="17" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="28" spans="1:4" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A28" s="17"/>
-      <c r="B28" s="17" t="s">
-        <v>16</v>
-      </c>
-      <c r="C28" s="20">
-        <v>-1E+20</v>
-      </c>
-      <c r="D28" s="4"/>
-    </row>
-    <row r="29" spans="1:4" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A29" s="17"/>
-      <c r="B29" s="17" t="s">
-        <v>17</v>
-      </c>
-      <c r="C29" s="19">
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="30" spans="1:4" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A30" s="17"/>
-      <c r="B30" s="17" t="s">
+    </row>
+    <row r="50" spans="1:4" ht="12" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A50" s="12"/>
+      <c r="B50" s="12" t="s">
         <v>18</v>
       </c>
-      <c r="C30" s="19">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="31" spans="1:4" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A31" s="17"/>
-      <c r="B31" s="17" t="s">
+      <c r="C50" s="7" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4" ht="12" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A51" s="12"/>
+      <c r="B51" s="12" t="s">
+        <v>29</v>
+      </c>
+      <c r="C51" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="D51" s="4"/>
+    </row>
+    <row r="52" spans="1:4" ht="12" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A52" s="12"/>
+      <c r="B52" s="12" t="s">
         <v>19</v>
       </c>
-      <c r="C31" s="17" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="32" spans="1:4" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="C32" s="4"/>
-    </row>
-    <row r="33" spans="1:4" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A33" t="s">
-        <v>25</v>
-      </c>
-      <c r="C33" s="4"/>
-    </row>
-    <row r="34" spans="1:4" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B34" t="s">
-        <v>8</v>
-      </c>
-      <c r="C34" s="6" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="35" spans="1:4" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B35" t="s">
-        <v>10</v>
-      </c>
-      <c r="C35" s="4" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="36" spans="1:4" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B36" t="s">
-        <v>3</v>
-      </c>
-      <c r="C36" s="5">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="37" spans="1:4" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B37" t="s">
-        <v>13</v>
-      </c>
-      <c r="C37" s="4"/>
-    </row>
-    <row r="38" spans="1:4" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B38" t="s">
-        <v>14</v>
-      </c>
-      <c r="C38" s="4" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="39" spans="1:4" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B39" t="s">
-        <v>16</v>
-      </c>
-      <c r="C39" s="7">
-        <v>-1E+20</v>
-      </c>
-      <c r="D39" s="4"/>
-    </row>
-    <row r="40" spans="1:4" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B40" t="s">
-        <v>17</v>
-      </c>
-      <c r="C40" s="8">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="41" spans="1:4" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B41" t="s">
-        <v>18</v>
-      </c>
-      <c r="C41" s="8">
-        <v>36000</v>
-      </c>
-    </row>
-    <row r="42" spans="1:4" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B42" t="s">
-        <v>19</v>
-      </c>
-      <c r="C42" s="4" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="43" spans="1:4" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="C43" s="4"/>
-    </row>
-    <row r="44" spans="1:4" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A44" t="s">
-        <v>27</v>
-      </c>
-      <c r="C44" s="4"/>
-    </row>
-    <row r="45" spans="1:4" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B45" t="s">
-        <v>8</v>
-      </c>
-      <c r="C45" s="6" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="46" spans="1:4" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B46" t="s">
-        <v>10</v>
-      </c>
-      <c r="C46" s="4" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="47" spans="1:4" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B47" t="s">
-        <v>3</v>
-      </c>
-      <c r="C47" s="4" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="48" spans="1:4" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B48" t="s">
-        <v>13</v>
-      </c>
-      <c r="C48" s="4"/>
-    </row>
-    <row r="49" spans="1:4" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B49" t="s">
-        <v>14</v>
-      </c>
-      <c r="C49" s="4" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="50" spans="1:4" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B50" t="s">
-        <v>16</v>
-      </c>
-      <c r="C50" s="7">
-        <v>-1E+20</v>
-      </c>
-    </row>
-    <row r="51" spans="1:4" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B51" t="s">
-        <v>30</v>
-      </c>
-      <c r="C51" s="4" t="s">
-        <v>31</v>
-      </c>
-      <c r="D51" s="4"/>
-    </row>
-    <row r="52" spans="1:4" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B52" t="s">
-        <v>19</v>
-      </c>
-      <c r="C52" s="4" t="s">
+      <c r="C52" s="5" t="s">
         <v>20</v>
       </c>
     </row>
@@ -1133,7 +1203,7 @@
     </row>
     <row r="54" spans="1:4" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A54" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C54" s="4"/>
     </row>
@@ -1141,7 +1211,7 @@
       <c r="B55" t="s">
         <v>8</v>
       </c>
-      <c r="C55" s="6" t="s">
+      <c r="C55" s="5" t="s">
         <v>22</v>
       </c>
     </row>
@@ -1158,610 +1228,691 @@
         <v>3</v>
       </c>
       <c r="C57" s="4" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="58" spans="1:4" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B58" t="s">
-        <v>13</v>
-      </c>
-      <c r="C58" s="4"/>
+        <v>14</v>
+      </c>
+      <c r="C58" s="4" t="s">
+        <v>33</v>
+      </c>
     </row>
     <row r="59" spans="1:4" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B59" t="s">
-        <v>14</v>
-      </c>
-      <c r="C59" s="4" t="s">
-        <v>34</v>
+        <v>16</v>
+      </c>
+      <c r="C59" s="6">
+        <v>-1E+20</v>
       </c>
     </row>
     <row r="60" spans="1:4" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B60" t="s">
-        <v>16</v>
-      </c>
-      <c r="C60" s="7">
-        <v>-1E+20</v>
+      <c r="A60" s="12"/>
+      <c r="B60" s="12" t="s">
+        <v>17</v>
+      </c>
+      <c r="C60" s="7" t="s">
+        <v>79</v>
       </c>
     </row>
     <row r="61" spans="1:4" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B61" t="s">
-        <v>30</v>
-      </c>
-      <c r="C61" s="4" t="s">
-        <v>31</v>
-      </c>
+      <c r="A61" s="12"/>
+      <c r="B61" s="12" t="s">
+        <v>18</v>
+      </c>
+      <c r="C61" s="7" t="s">
+        <v>79</v>
+      </c>
+      <c r="D61" s="4"/>
     </row>
     <row r="62" spans="1:4" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B62" t="s">
+        <v>29</v>
+      </c>
+      <c r="C62" s="4" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="63" spans="1:4" ht="12" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B63" t="s">
         <v>19</v>
       </c>
-      <c r="C62" s="4" t="s">
+      <c r="C63" s="4" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="63" spans="1:4" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="C63" s="4"/>
-      <c r="D63" s="4"/>
-    </row>
     <row r="64" spans="1:4" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A64" t="s">
+      <c r="C64" s="4"/>
+    </row>
+    <row r="65" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A65" s="12" t="s">
+        <v>34</v>
+      </c>
+      <c r="B65" s="12"/>
+      <c r="C65" s="5"/>
+    </row>
+    <row r="66" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A66" s="12"/>
+      <c r="B66" s="12" t="s">
+        <v>8</v>
+      </c>
+      <c r="C66" s="5" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="67" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A67" s="12"/>
+      <c r="B67" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="C67" s="5" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="68" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A68" s="12"/>
+      <c r="B68" s="12" t="s">
+        <v>3</v>
+      </c>
+      <c r="C68" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="C64" s="4"/>
-    </row>
-    <row r="65" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B65" t="s">
+    </row>
+    <row r="69" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A69" s="12"/>
+      <c r="B69" s="12" t="s">
+        <v>14</v>
+      </c>
+      <c r="C69" s="5" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="70" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A70" s="12"/>
+      <c r="B70" s="12" t="s">
+        <v>16</v>
+      </c>
+      <c r="C70" s="15">
+        <v>-1E+20</v>
+      </c>
+    </row>
+    <row r="71" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A71" s="12"/>
+      <c r="B71" s="12" t="s">
+        <v>17</v>
+      </c>
+      <c r="C71" s="7" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="72" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A72" s="12"/>
+      <c r="B72" s="12" t="s">
+        <v>18</v>
+      </c>
+      <c r="C72" s="7" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="73" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A73" s="12"/>
+      <c r="B73" s="12" t="s">
+        <v>29</v>
+      </c>
+      <c r="C73" s="5" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="74" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A74" s="12"/>
+      <c r="B74" s="12" t="s">
+        <v>19</v>
+      </c>
+      <c r="C74" s="5" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="75" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A75" s="12"/>
+      <c r="B75" s="12"/>
+      <c r="C75" s="5"/>
+    </row>
+    <row r="76" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A76" s="12" t="s">
+        <v>37</v>
+      </c>
+      <c r="B76" s="12"/>
+      <c r="C76" s="5"/>
+    </row>
+    <row r="77" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A77" s="12"/>
+      <c r="B77" s="12" t="s">
         <v>8</v>
       </c>
-      <c r="C65" s="6" t="s">
+      <c r="C77" s="5" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="66" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B66" t="s">
+    <row r="78" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A78" s="12"/>
+      <c r="B78" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="C66" s="4" t="s">
+      <c r="C78" s="5" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="67" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B67" t="s">
+    <row r="79" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A79" s="12"/>
+      <c r="B79" s="12" t="s">
         <v>3</v>
       </c>
-      <c r="C67" s="4" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="68" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B68" t="s">
+      <c r="C79" s="5" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="80" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A80" s="12"/>
+      <c r="B80" s="12" t="s">
         <v>13</v>
       </c>
-      <c r="C68" s="4"/>
-    </row>
-    <row r="69" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B69" t="s">
+      <c r="C80" s="5" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="81" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A81" s="12"/>
+      <c r="B81" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="C69" s="4" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="70" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B70" t="s">
+      <c r="C81" s="5" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="82" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A82" s="12"/>
+      <c r="B82" s="12" t="s">
         <v>16</v>
       </c>
-      <c r="C70" s="7">
+      <c r="C82" s="15">
         <v>-1E+20</v>
       </c>
     </row>
-    <row r="71" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B71" t="s">
+    <row r="83" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A83" s="12"/>
+      <c r="B83" s="12" t="s">
+        <v>17</v>
+      </c>
+      <c r="C83" s="7" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="84" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A84" s="12"/>
+      <c r="B84" s="12" t="s">
+        <v>18</v>
+      </c>
+      <c r="C84" s="7" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="85" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A85" s="12"/>
+      <c r="B85" s="12" t="s">
+        <v>29</v>
+      </c>
+      <c r="C85" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="C71" s="4" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="72" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B72" t="s">
+    </row>
+    <row r="86" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A86" s="12"/>
+      <c r="B86" s="12" t="s">
         <v>19</v>
       </c>
-      <c r="C72" s="4" t="s">
+      <c r="C86" s="5" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="73" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="C73" s="4"/>
-    </row>
-    <row r="74" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A74" t="s">
+    <row r="87" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A87" s="12"/>
+      <c r="B87" s="12"/>
+      <c r="C87" s="5"/>
+    </row>
+    <row r="88" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A88" s="12" t="s">
+        <v>40</v>
+      </c>
+      <c r="B88" s="12"/>
+      <c r="C88" s="5"/>
+    </row>
+    <row r="89" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A89" s="12"/>
+      <c r="B89" s="12" t="s">
+        <v>8</v>
+      </c>
+      <c r="C89" s="5" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="90" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A90" s="12"/>
+      <c r="B90" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="C90" s="5" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="91" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A91" s="12"/>
+      <c r="B91" s="12" t="s">
+        <v>3</v>
+      </c>
+      <c r="C91" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="C74" s="4"/>
-    </row>
-    <row r="75" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B75" t="s">
+    </row>
+    <row r="92" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A92" s="12"/>
+      <c r="B92" s="12" t="s">
+        <v>13</v>
+      </c>
+      <c r="C92" s="5" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="93" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A93" s="12"/>
+      <c r="B93" s="12" t="s">
+        <v>14</v>
+      </c>
+      <c r="C93" s="5" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="94" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A94" s="12"/>
+      <c r="B94" s="12" t="s">
+        <v>16</v>
+      </c>
+      <c r="C94" s="15">
+        <v>-1E+20</v>
+      </c>
+    </row>
+    <row r="95" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A95" s="12"/>
+      <c r="B95" s="12" t="s">
+        <v>17</v>
+      </c>
+      <c r="C95" s="7" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="96" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A96" s="12"/>
+      <c r="B96" s="12" t="s">
+        <v>18</v>
+      </c>
+      <c r="C96" s="7" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="97" spans="1:4" ht="12" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A97" s="12"/>
+      <c r="B97" s="12" t="s">
+        <v>29</v>
+      </c>
+      <c r="C97" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="D97" s="4"/>
+    </row>
+    <row r="98" spans="1:4" ht="12" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A98" s="12"/>
+      <c r="B98" s="12" t="s">
+        <v>19</v>
+      </c>
+      <c r="C98" s="5" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="99" spans="1:4" ht="12" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="C99" s="4"/>
+    </row>
+    <row r="100" spans="1:4" ht="12" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A100" s="12" t="s">
+        <v>42</v>
+      </c>
+      <c r="B100" s="12"/>
+      <c r="C100" s="5"/>
+    </row>
+    <row r="101" spans="1:4" ht="12" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A101" s="12"/>
+      <c r="B101" s="12" t="s">
         <v>8</v>
       </c>
-      <c r="C75" s="6" t="s">
+      <c r="C101" s="5" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="76" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B76" t="s">
+    <row r="102" spans="1:4" ht="12" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A102" s="12"/>
+      <c r="B102" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="C76" s="4" t="s">
+      <c r="C102" s="5" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="77" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B77" t="s">
+    <row r="103" spans="1:4" ht="12" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A103" s="12"/>
+      <c r="B103" s="12" t="s">
         <v>3</v>
       </c>
-      <c r="C77" s="4" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="78" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B78" t="s">
-        <v>13</v>
-      </c>
-      <c r="C78" s="4" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="79" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B79" t="s">
+      <c r="C103" s="5" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="104" spans="1:4" ht="12" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A104" s="12"/>
+      <c r="B104" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="C79" s="4" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="80" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B80" t="s">
+      <c r="C104" s="5" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="105" spans="1:4" ht="12" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A105" s="12"/>
+      <c r="B105" s="12" t="s">
         <v>16</v>
       </c>
-      <c r="C80" s="7">
+      <c r="C105" s="15">
         <v>-1E+20</v>
       </c>
     </row>
-    <row r="81" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B81" t="s">
+    <row r="106" spans="1:4" ht="12" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A106" s="12"/>
+      <c r="B106" s="12" t="s">
+        <v>17</v>
+      </c>
+      <c r="C106" s="7" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="107" spans="1:4" ht="12" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A107" s="12"/>
+      <c r="B107" s="12" t="s">
+        <v>18</v>
+      </c>
+      <c r="C107" s="7" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="108" spans="1:4" ht="12" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A108" s="12"/>
+      <c r="B108" s="12" t="s">
+        <v>29</v>
+      </c>
+      <c r="C108" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="C81" s="4" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="82" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B82" t="s">
+    </row>
+    <row r="109" spans="1:4" ht="12" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A109" s="12"/>
+      <c r="B109" s="12" t="s">
         <v>19</v>
       </c>
-      <c r="C82" s="4" t="s">
+      <c r="C109" s="5" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="83" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="C83" s="4"/>
-    </row>
-    <row r="84" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A84" t="s">
-        <v>41</v>
-      </c>
-      <c r="C84" s="4"/>
-    </row>
-    <row r="85" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B85" t="s">
+      <c r="D109" s="4"/>
+    </row>
+    <row r="110" spans="1:4" ht="12" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A110" s="12"/>
+      <c r="B110" s="12"/>
+      <c r="C110" s="5"/>
+    </row>
+    <row r="111" spans="1:4" ht="12" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A111" s="12" t="s">
+        <v>45</v>
+      </c>
+      <c r="B111" s="12"/>
+      <c r="C111" s="5"/>
+    </row>
+    <row r="112" spans="1:4" ht="12" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A112" s="12"/>
+      <c r="B112" s="12" t="s">
         <v>8</v>
       </c>
-      <c r="C85" s="6" t="s">
+      <c r="C112" s="5" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="86" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B86" t="s">
+    <row r="113" spans="1:4" ht="12" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A113" s="12"/>
+      <c r="B113" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="C86" s="4" t="s">
+      <c r="C113" s="5" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="87" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B87" t="s">
+    <row r="114" spans="1:4" ht="12" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A114" s="12"/>
+      <c r="B114" s="12" t="s">
         <v>3</v>
       </c>
-      <c r="C87" s="4" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="88" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B88" t="s">
-        <v>13</v>
-      </c>
-      <c r="C88" s="4" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="89" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B89" t="s">
+      <c r="C114" s="5" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="115" spans="1:4" ht="12" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A115" s="12"/>
+      <c r="B115" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="C89" s="4" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="90" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B90" t="s">
+      <c r="C115" s="5" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="116" spans="1:4" ht="12" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A116" s="12"/>
+      <c r="B116" s="12" t="s">
         <v>16</v>
       </c>
-      <c r="C90" s="7">
+      <c r="C116" s="15">
         <v>-1E+20</v>
       </c>
     </row>
-    <row r="91" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B91" t="s">
+    <row r="117" spans="1:4" ht="12" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A117" s="12"/>
+      <c r="B117" s="12" t="s">
+        <v>17</v>
+      </c>
+      <c r="C117" s="7" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="118" spans="1:4" ht="12" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A118" s="12"/>
+      <c r="B118" s="12" t="s">
+        <v>18</v>
+      </c>
+      <c r="C118" s="7" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="119" spans="1:4" ht="12" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A119" s="12"/>
+      <c r="B119" s="12" t="s">
+        <v>29</v>
+      </c>
+      <c r="C119" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="C91" s="4" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="92" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B92" t="s">
+    </row>
+    <row r="120" spans="1:4" ht="12" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A120" s="12"/>
+      <c r="B120" s="12" t="s">
         <v>19</v>
       </c>
-      <c r="C92" s="4" t="s">
+      <c r="C120" s="5" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="93" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="C93" s="4"/>
-    </row>
-    <row r="94" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A94" t="s">
-        <v>43</v>
-      </c>
-      <c r="C94" s="4"/>
-    </row>
-    <row r="95" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B95" t="s">
+    <row r="121" spans="1:4" ht="12" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="C121" s="5"/>
+      <c r="D121" s="4"/>
+    </row>
+    <row r="122" spans="1:4" ht="12" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A122" s="12" t="s">
+        <v>47</v>
+      </c>
+      <c r="B122" s="12"/>
+      <c r="C122" s="5"/>
+    </row>
+    <row r="123" spans="1:4" ht="12" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A123" s="12"/>
+      <c r="B123" s="12" t="s">
         <v>8</v>
       </c>
-      <c r="C95" s="6" t="s">
+      <c r="C123" s="5" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="96" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B96" t="s">
+    <row r="124" spans="1:4" ht="12" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A124" s="12"/>
+      <c r="B124" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="C96" s="4" t="s">
+      <c r="C124" s="5" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="97" spans="1:4" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B97" t="s">
+    <row r="125" spans="1:4" ht="12" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A125" s="12"/>
+      <c r="B125" s="12" t="s">
         <v>3</v>
       </c>
-      <c r="C97" s="4" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="98" spans="1:4" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B98" t="s">
-        <v>13</v>
-      </c>
-      <c r="C98" s="4"/>
-    </row>
-    <row r="99" spans="1:4" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B99" t="s">
+      <c r="C125" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="126" spans="1:4" ht="12" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A126" s="12"/>
+      <c r="B126" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="C99" s="4" t="s">
-        <v>45</v>
-      </c>
-      <c r="D99" s="4"/>
-    </row>
-    <row r="100" spans="1:4" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B100" t="s">
+      <c r="C126" s="5" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="127" spans="1:4" ht="12" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A127" s="12"/>
+      <c r="B127" s="12" t="s">
         <v>16</v>
       </c>
-      <c r="C100" s="7">
+      <c r="C127" s="15">
         <v>-1E+20</v>
       </c>
     </row>
-    <row r="101" spans="1:4" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B101" t="s">
+    <row r="128" spans="1:4" ht="12" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A128" s="12"/>
+      <c r="B128" s="12" t="s">
+        <v>17</v>
+      </c>
+      <c r="C128" s="7" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="129" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A129" s="12"/>
+      <c r="B129" s="12" t="s">
+        <v>18</v>
+      </c>
+      <c r="C129" s="7" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="130" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A130" s="12"/>
+      <c r="B130" s="12" t="s">
+        <v>29</v>
+      </c>
+      <c r="C130" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="C101" s="4" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="102" spans="1:4" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B102" t="s">
+    </row>
+    <row r="131" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A131" s="12"/>
+      <c r="B131" s="12" t="s">
         <v>19</v>
       </c>
-      <c r="C102" s="4" t="s">
+      <c r="C131" s="5" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="103" spans="1:4" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="C103" s="4"/>
-    </row>
-    <row r="104" spans="1:4" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A104" t="s">
-        <v>46</v>
-      </c>
-      <c r="C104" s="4"/>
-    </row>
-    <row r="105" spans="1:4" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B105" t="s">
+    <row r="132" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="C132" s="4"/>
+    </row>
+    <row r="133" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A133" s="13" t="s">
+        <v>49</v>
+      </c>
+      <c r="B133" s="13"/>
+      <c r="C133" s="5"/>
+    </row>
+    <row r="134" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A134" s="13"/>
+      <c r="B134" s="13" t="s">
         <v>8</v>
       </c>
-      <c r="C105" s="6" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="106" spans="1:4" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B106" t="s">
+      <c r="C134" s="5" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="135" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A135" s="13"/>
+      <c r="B135" s="13" t="s">
         <v>10</v>
       </c>
-      <c r="C106" s="4" t="s">
+      <c r="C135" s="5" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="107" spans="1:4" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B107" t="s">
+    <row r="136" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A136" s="13"/>
+      <c r="B136" s="13" t="s">
         <v>3</v>
       </c>
-      <c r="C107" s="4" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="108" spans="1:4" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B108" t="s">
-        <v>13</v>
-      </c>
-      <c r="C108" s="4"/>
-    </row>
-    <row r="109" spans="1:4" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B109" t="s">
+      <c r="C136" s="7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="137" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A137" s="13"/>
+      <c r="B137" s="13" t="s">
         <v>14</v>
       </c>
-      <c r="C109" s="4" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="110" spans="1:4" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B110" t="s">
-        <v>16</v>
-      </c>
-      <c r="C110" s="7">
-        <v>-1E+20</v>
-      </c>
-    </row>
-    <row r="111" spans="1:4" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B111" t="s">
-        <v>30</v>
-      </c>
-      <c r="C111" s="4" t="s">
-        <v>31</v>
-      </c>
-      <c r="D111" s="4"/>
-    </row>
-    <row r="112" spans="1:4" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B112" t="s">
-        <v>19</v>
-      </c>
-      <c r="C112" s="4" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="113" spans="1:4" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="C113" s="4"/>
-    </row>
-    <row r="114" spans="1:4" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A114" t="s">
-        <v>48</v>
-      </c>
-      <c r="C114" s="4"/>
-    </row>
-    <row r="115" spans="1:4" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B115" t="s">
-        <v>8</v>
-      </c>
-      <c r="C115" s="6" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="116" spans="1:4" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B116" t="s">
-        <v>10</v>
-      </c>
-      <c r="C116" s="4" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="117" spans="1:4" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B117" t="s">
-        <v>3</v>
-      </c>
-      <c r="C117" s="4">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="118" spans="1:4" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B118" t="s">
-        <v>13</v>
-      </c>
-      <c r="C118" s="4"/>
-    </row>
-    <row r="119" spans="1:4" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B119" t="s">
-        <v>14</v>
-      </c>
-      <c r="C119" s="4" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="120" spans="1:4" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B120" t="s">
-        <v>16</v>
-      </c>
-      <c r="C120" s="7">
-        <v>-1E+20</v>
-      </c>
-    </row>
-    <row r="121" spans="1:4" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B121" t="s">
-        <v>30</v>
-      </c>
-      <c r="C121" s="4" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="122" spans="1:4" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B122" t="s">
-        <v>19</v>
-      </c>
-      <c r="C122" s="4" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="123" spans="1:4" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="C123" s="4"/>
-      <c r="D123" s="4"/>
-    </row>
-    <row r="124" spans="1:4" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A124" s="9" t="s">
-        <v>50</v>
-      </c>
-      <c r="B124" s="9"/>
-      <c r="C124" s="10"/>
-    </row>
-    <row r="125" spans="1:4" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A125" s="9"/>
-      <c r="B125" s="9" t="s">
-        <v>8</v>
-      </c>
-      <c r="C125" s="10" t="s">
+      <c r="C137" s="5" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="126" spans="1:4" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A126" s="9"/>
-      <c r="B126" s="9" t="s">
-        <v>10</v>
-      </c>
-      <c r="C126" s="10" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="127" spans="1:4" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A127" s="9"/>
-      <c r="B127" s="9" t="s">
-        <v>3</v>
-      </c>
-      <c r="C127" s="8">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="128" spans="1:4" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A128" s="9"/>
-      <c r="B128" s="9" t="s">
-        <v>13</v>
-      </c>
-      <c r="C128" s="10"/>
-    </row>
-    <row r="129" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A129" s="9"/>
-      <c r="B129" s="9" t="s">
-        <v>14</v>
-      </c>
-      <c r="C129" s="10" t="s">
+    <row r="138" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A138" s="13"/>
+      <c r="B138" s="13" t="s">
         <v>52</v>
       </c>
-    </row>
-    <row r="130" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A130" s="9"/>
-      <c r="B130" s="9" t="s">
-        <v>53</v>
-      </c>
-      <c r="C130" s="11" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="131" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A131" s="9"/>
-      <c r="B131" s="12" t="s">
-        <v>54</v>
-      </c>
-      <c r="C131" s="13" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="132" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A132" s="9"/>
-      <c r="B132" s="9"/>
-      <c r="C132" s="10"/>
-    </row>
-    <row r="133" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A133" s="9" t="s">
-        <v>55</v>
-      </c>
-      <c r="B133" s="9"/>
-      <c r="C133" s="10"/>
-    </row>
-    <row r="134" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A134" s="9"/>
-      <c r="B134" s="9" t="s">
-        <v>8</v>
-      </c>
-      <c r="C134" s="10" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="135" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A135" s="9"/>
-      <c r="B135" s="9" t="s">
-        <v>10</v>
-      </c>
-      <c r="C135" s="10" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="136" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A136" s="9"/>
-      <c r="B136" s="9" t="s">
-        <v>3</v>
-      </c>
-      <c r="C136" s="8">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="137" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A137" s="9"/>
-      <c r="B137" s="9" t="s">
-        <v>13</v>
-      </c>
-      <c r="C137" s="10"/>
-    </row>
-    <row r="138" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A138" s="9"/>
-      <c r="B138" s="9" t="s">
-        <v>14</v>
-      </c>
       <c r="C138" s="10" t="s">
-        <v>56</v>
+        <v>72</v>
       </c>
     </row>
     <row r="139" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A139" s="9"/>
-      <c r="B139" s="9" t="s">
+      <c r="A139" s="13"/>
+      <c r="B139" s="17" t="s">
         <v>53</v>
       </c>
       <c r="C139" s="11" t="s">
@@ -1769,675 +1920,677 @@
       </c>
     </row>
     <row r="140" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A140" s="9"/>
-      <c r="B140" s="12" t="s">
+      <c r="A140" s="13"/>
+      <c r="B140" s="13"/>
+      <c r="C140" s="5"/>
+    </row>
+    <row r="141" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A141" s="13" t="s">
         <v>54</v>
       </c>
-      <c r="C140" s="13" t="s">
+      <c r="B141" s="13"/>
+      <c r="C141" s="5"/>
+    </row>
+    <row r="142" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A142" s="13"/>
+      <c r="B142" s="13" t="s">
+        <v>8</v>
+      </c>
+      <c r="C142" s="5" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="143" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A143" s="13"/>
+      <c r="B143" s="13" t="s">
+        <v>10</v>
+      </c>
+      <c r="C143" s="5" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="144" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A144" s="13"/>
+      <c r="B144" s="13" t="s">
+        <v>3</v>
+      </c>
+      <c r="C144" s="7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="145" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A145" s="13"/>
+      <c r="B145" s="13" t="s">
+        <v>13</v>
+      </c>
+      <c r="C145" s="5"/>
+    </row>
+    <row r="146" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A146" s="13"/>
+      <c r="B146" s="13" t="s">
+        <v>14</v>
+      </c>
+      <c r="C146" s="5" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="147" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A147" s="13"/>
+      <c r="B147" s="13" t="s">
+        <v>52</v>
+      </c>
+      <c r="C147" s="10" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="148" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A148" s="13"/>
+      <c r="B148" s="17" t="s">
+        <v>53</v>
+      </c>
+      <c r="C148" s="11" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="149" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A149" s="13"/>
+      <c r="B149" s="13"/>
+      <c r="C149" s="5"/>
+    </row>
+    <row r="150" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A150" s="13" t="s">
+        <v>56</v>
+      </c>
+      <c r="B150" s="13"/>
+      <c r="C150" s="5"/>
+    </row>
+    <row r="151" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A151" s="13"/>
+      <c r="B151" s="13" t="s">
+        <v>8</v>
+      </c>
+      <c r="C151" s="5" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="152" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A152" s="13"/>
+      <c r="B152" s="13" t="s">
+        <v>10</v>
+      </c>
+      <c r="C152" s="5" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="153" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A153" s="13"/>
+      <c r="B153" s="13" t="s">
+        <v>3</v>
+      </c>
+      <c r="C153" s="7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="154" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A154" s="13"/>
+      <c r="B154" s="13" t="s">
+        <v>14</v>
+      </c>
+      <c r="C154" s="5" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="155" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A155" s="13"/>
+      <c r="B155" s="13" t="s">
+        <v>52</v>
+      </c>
+      <c r="C155" s="10" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="156" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A156" s="13"/>
+      <c r="B156" s="17" t="s">
+        <v>53</v>
+      </c>
+      <c r="C156" s="11" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="157" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A157" s="13"/>
+      <c r="B157" s="13"/>
+      <c r="C157" s="5"/>
+    </row>
+    <row r="158" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A158" s="13" t="s">
+        <v>58</v>
+      </c>
+      <c r="B158" s="13"/>
+      <c r="C158" s="5"/>
+    </row>
+    <row r="159" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A159" s="13"/>
+      <c r="B159" s="13" t="s">
+        <v>8</v>
+      </c>
+      <c r="C159" s="5" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="160" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A160" s="13"/>
+      <c r="B160" s="13" t="s">
+        <v>10</v>
+      </c>
+      <c r="C160" s="5" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="161" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A161" s="13"/>
+      <c r="B161" s="13" t="s">
+        <v>3</v>
+      </c>
+      <c r="C161" s="7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="162" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A162" s="13"/>
+      <c r="B162" s="13" t="s">
+        <v>14</v>
+      </c>
+      <c r="C162" s="5" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="163" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A163" s="13"/>
+      <c r="B163" s="13" t="s">
+        <v>52</v>
+      </c>
+      <c r="C163" s="10" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="164" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A164" s="13"/>
+      <c r="B164" s="17" t="s">
+        <v>53</v>
+      </c>
+      <c r="C164" s="11" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="165" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A165" s="8"/>
+      <c r="B165" s="8"/>
+      <c r="C165" s="9"/>
+    </row>
+    <row r="166" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A166" s="13" t="s">
         <v>74</v>
       </c>
-    </row>
-    <row r="141" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A141" s="9"/>
-      <c r="B141" s="9"/>
-      <c r="C141" s="10"/>
-    </row>
-    <row r="142" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A142" s="9" t="s">
-        <v>57</v>
-      </c>
-      <c r="B142" s="9"/>
-      <c r="C142" s="10"/>
-    </row>
-    <row r="143" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A143" s="9"/>
-      <c r="B143" s="9" t="s">
+      <c r="B166" s="13"/>
+      <c r="C166" s="5"/>
+    </row>
+    <row r="167" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A167" s="13"/>
+      <c r="B167" s="13" t="s">
         <v>8</v>
       </c>
-      <c r="C143" s="10" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="144" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A144" s="9"/>
-      <c r="B144" s="9" t="s">
+      <c r="C167" s="5" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="168" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A168" s="13"/>
+      <c r="B168" s="13" t="s">
         <v>10</v>
       </c>
-      <c r="C144" s="10" t="s">
+      <c r="C168" s="5" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="145" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A145" s="9"/>
-      <c r="B145" s="9" t="s">
+    <row r="169" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A169" s="13"/>
+      <c r="B169" s="13" t="s">
         <v>3</v>
       </c>
-      <c r="C145" s="8">
+      <c r="C169" s="7">
         <v>1</v>
       </c>
     </row>
-    <row r="146" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A146" s="9"/>
-      <c r="B146" s="9" t="s">
-        <v>13</v>
-      </c>
-      <c r="C146" s="10"/>
-    </row>
-    <row r="147" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A147" s="9"/>
-      <c r="B147" s="9" t="s">
+    <row r="170" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A170" s="13"/>
+      <c r="B170" s="13" t="s">
         <v>14</v>
       </c>
-      <c r="C147" s="10" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="148" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A148" s="9"/>
-      <c r="B148" s="9" t="s">
+      <c r="C170" s="5" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="171" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A171" s="13"/>
+      <c r="B171" s="13" t="s">
+        <v>52</v>
+      </c>
+      <c r="C171" s="10" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="172" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A172" s="13"/>
+      <c r="B172" s="17" t="s">
         <v>53</v>
       </c>
-      <c r="C148" s="11" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="149" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A149" s="9"/>
-      <c r="B149" s="12" t="s">
-        <v>54</v>
-      </c>
-      <c r="C149" s="13" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="150" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A150" s="9"/>
-      <c r="B150" s="9"/>
-      <c r="C150" s="10"/>
-    </row>
-    <row r="151" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A151" s="9" t="s">
-        <v>59</v>
-      </c>
-      <c r="B151" s="9"/>
-      <c r="C151" s="10"/>
-    </row>
-    <row r="152" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A152" s="9"/>
-      <c r="B152" s="9" t="s">
+      <c r="C172" s="11" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="173" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A173" s="13"/>
+      <c r="B173" s="13"/>
+      <c r="C173" s="5"/>
+    </row>
+    <row r="174" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A174" s="13" t="s">
+        <v>75</v>
+      </c>
+      <c r="B174" s="13"/>
+      <c r="C174" s="5"/>
+    </row>
+    <row r="175" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A175" s="13"/>
+      <c r="B175" s="13" t="s">
         <v>8</v>
       </c>
-      <c r="C152" s="10" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="153" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A153" s="9"/>
-      <c r="B153" s="9" t="s">
+      <c r="C175" s="5" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="176" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A176" s="13"/>
+      <c r="B176" s="13" t="s">
         <v>10</v>
       </c>
-      <c r="C153" s="10" t="s">
+      <c r="C176" s="5" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="154" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A154" s="9"/>
-      <c r="B154" s="9" t="s">
+    <row r="177" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A177" s="13"/>
+      <c r="B177" s="13" t="s">
         <v>3</v>
       </c>
-      <c r="C154" s="8">
+      <c r="C177" s="7">
         <v>1</v>
       </c>
     </row>
-    <row r="155" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A155" s="9"/>
-      <c r="B155" s="9" t="s">
-        <v>13</v>
-      </c>
-      <c r="C155" s="10"/>
-    </row>
-    <row r="156" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A156" s="9"/>
-      <c r="B156" s="9" t="s">
+    <row r="178" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A178" s="13"/>
+      <c r="B178" s="13" t="s">
         <v>14</v>
       </c>
-      <c r="C156" s="10" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="157" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A157" s="9"/>
-      <c r="B157" s="9" t="s">
+      <c r="C178" s="5" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="179" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A179" s="13"/>
+      <c r="B179" s="13" t="s">
+        <v>52</v>
+      </c>
+      <c r="C179" s="10" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="180" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A180" s="13"/>
+      <c r="B180" s="17" t="s">
         <v>53</v>
       </c>
-      <c r="C157" s="11" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="158" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A158" s="9"/>
-      <c r="B158" s="12" t="s">
-        <v>54</v>
-      </c>
-      <c r="C158" s="13" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="159" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A159" s="9"/>
-      <c r="B159" s="9"/>
-      <c r="C159" s="10"/>
-    </row>
-    <row r="160" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A160" s="16" t="s">
-        <v>77</v>
-      </c>
-      <c r="B160" s="9"/>
-      <c r="C160" s="10"/>
-    </row>
-    <row r="161" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A161" s="9"/>
-      <c r="B161" s="9" t="s">
+      <c r="C180" s="11" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="181" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A181" s="13"/>
+      <c r="B181" s="13"/>
+      <c r="C181" s="5"/>
+    </row>
+    <row r="182" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A182" s="13" t="s">
+        <v>62</v>
+      </c>
+      <c r="B182" s="13"/>
+      <c r="C182" s="5"/>
+    </row>
+    <row r="183" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A183" s="13"/>
+      <c r="B183" s="13" t="s">
         <v>8</v>
       </c>
-      <c r="C161" s="10" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="162" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A162" s="9"/>
-      <c r="B162" s="9" t="s">
+      <c r="C183" s="5" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="184" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A184" s="13"/>
+      <c r="B184" s="13" t="s">
         <v>10</v>
       </c>
-      <c r="C162" s="10" t="s">
+      <c r="C184" s="5" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="163" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A163" s="9"/>
-      <c r="B163" s="9" t="s">
+    <row r="185" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A185" s="13"/>
+      <c r="B185" s="13" t="s">
         <v>3</v>
       </c>
-      <c r="C163" s="8">
+      <c r="C185" s="7">
         <v>1</v>
       </c>
     </row>
-    <row r="164" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A164" s="9"/>
-      <c r="B164" s="9" t="s">
-        <v>13</v>
-      </c>
-      <c r="C164" s="10"/>
-    </row>
-    <row r="165" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A165" s="9"/>
-      <c r="B165" s="9" t="s">
+    <row r="186" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A186" s="13"/>
+      <c r="B186" s="13" t="s">
         <v>14</v>
       </c>
-      <c r="C165" s="10" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="166" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A166" s="9"/>
-      <c r="B166" s="9" t="s">
+      <c r="C186" s="5" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="187" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A187" s="13"/>
+      <c r="B187" s="13" t="s">
+        <v>52</v>
+      </c>
+      <c r="C187" s="10" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="188" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A188" s="13"/>
+      <c r="B188" s="17" t="s">
         <v>53</v>
       </c>
-      <c r="C166" s="11" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="167" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A167" s="9"/>
-      <c r="B167" s="12" t="s">
-        <v>54</v>
-      </c>
-      <c r="C167" s="13" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="168" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A168" s="9"/>
-      <c r="B168" s="9"/>
-      <c r="C168" s="10"/>
-    </row>
-    <row r="169" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A169" s="16" t="s">
-        <v>78</v>
-      </c>
-      <c r="B169" s="9"/>
-      <c r="C169" s="10"/>
-    </row>
-    <row r="170" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A170" s="9"/>
-      <c r="B170" s="9" t="s">
+      <c r="C188" s="11" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="189" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A189" s="13"/>
+      <c r="B189" s="13"/>
+      <c r="C189" s="5"/>
+    </row>
+    <row r="190" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A190" s="13" t="s">
+        <v>64</v>
+      </c>
+      <c r="B190" s="13"/>
+      <c r="C190" s="5"/>
+    </row>
+    <row r="191" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A191" s="13"/>
+      <c r="B191" s="13" t="s">
         <v>8</v>
       </c>
-      <c r="C170" s="10" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="171" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A171" s="9"/>
-      <c r="B171" s="9" t="s">
+      <c r="C191" s="5" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="192" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A192" s="13"/>
+      <c r="B192" s="13" t="s">
         <v>10</v>
       </c>
-      <c r="C171" s="10" t="s">
+      <c r="C192" s="5" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="172" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A172" s="9"/>
-      <c r="B172" s="9" t="s">
+    <row r="193" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A193" s="13"/>
+      <c r="B193" s="13" t="s">
         <v>3</v>
       </c>
-      <c r="C172" s="8">
+      <c r="C193" s="7">
         <v>1</v>
       </c>
     </row>
-    <row r="173" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A173" s="9"/>
-      <c r="B173" s="9" t="s">
-        <v>13</v>
-      </c>
-      <c r="C173" s="10"/>
-    </row>
-    <row r="174" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A174" s="9"/>
-      <c r="B174" s="9" t="s">
+    <row r="194" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A194" s="13"/>
+      <c r="B194" s="13" t="s">
         <v>14</v>
       </c>
-      <c r="C174" s="10" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="175" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A175" s="9"/>
-      <c r="B175" s="9" t="s">
+      <c r="C194" s="5" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="195" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A195" s="13"/>
+      <c r="B195" s="13" t="s">
+        <v>52</v>
+      </c>
+      <c r="C195" s="10" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="196" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A196" s="13"/>
+      <c r="B196" s="17" t="s">
         <v>53</v>
       </c>
-      <c r="C175" s="11" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="176" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A176" s="9"/>
-      <c r="B176" s="12" t="s">
-        <v>54</v>
-      </c>
-      <c r="C176" s="13" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="177" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A177" s="9"/>
-      <c r="B177" s="9"/>
-      <c r="C177" s="10"/>
-    </row>
-    <row r="178" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A178" s="16" t="s">
-        <v>63</v>
-      </c>
-      <c r="B178" s="9"/>
-      <c r="C178" s="10"/>
-    </row>
-    <row r="179" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A179" s="9"/>
-      <c r="B179" s="9" t="s">
+      <c r="C196" s="11" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="197" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A197" s="13"/>
+      <c r="B197" s="13"/>
+      <c r="C197" s="5"/>
+    </row>
+    <row r="198" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A198" s="13" t="s">
+        <v>66</v>
+      </c>
+      <c r="B198" s="13"/>
+      <c r="C198" s="5"/>
+    </row>
+    <row r="199" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A199" s="13"/>
+      <c r="B199" s="13" t="s">
         <v>8</v>
       </c>
-      <c r="C179" s="10" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="180" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A180" s="9"/>
-      <c r="B180" s="9" t="s">
+      <c r="C199" s="5" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="200" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A200" s="13"/>
+      <c r="B200" s="13" t="s">
         <v>10</v>
       </c>
-      <c r="C180" s="10" t="s">
+      <c r="C200" s="5" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="181" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A181" s="9"/>
-      <c r="B181" s="9" t="s">
+    <row r="201" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A201" s="13"/>
+      <c r="B201" s="13" t="s">
         <v>3</v>
       </c>
-      <c r="C181" s="8">
+      <c r="C201" s="7">
         <v>1</v>
       </c>
     </row>
-    <row r="182" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A182" s="9"/>
-      <c r="B182" s="9" t="s">
-        <v>13</v>
-      </c>
-      <c r="C182" s="10"/>
-    </row>
-    <row r="183" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A183" s="9"/>
-      <c r="B183" s="9" t="s">
+    <row r="202" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A202" s="13"/>
+      <c r="B202" s="13" t="s">
         <v>14</v>
       </c>
-      <c r="C183" s="10" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="184" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A184" s="9"/>
-      <c r="B184" s="9" t="s">
+      <c r="C202" s="5" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="203" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A203" s="13"/>
+      <c r="B203" s="13" t="s">
+        <v>52</v>
+      </c>
+      <c r="C203" s="10" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="204" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A204" s="13"/>
+      <c r="B204" s="17" t="s">
         <v>53</v>
       </c>
-      <c r="C184" s="11" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="185" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A185" s="9"/>
-      <c r="B185" s="12" t="s">
-        <v>54</v>
-      </c>
-      <c r="C185" s="13" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="186" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A186" s="9"/>
-      <c r="B186" s="9"/>
-      <c r="C186" s="10"/>
-    </row>
-    <row r="187" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A187" s="9" t="s">
-        <v>65</v>
-      </c>
-      <c r="B187" s="9"/>
-      <c r="C187" s="10"/>
-    </row>
-    <row r="188" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A188" s="9"/>
-      <c r="B188" s="9" t="s">
+      <c r="C204" s="11" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="205" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A205" s="13"/>
+      <c r="B205" s="13"/>
+      <c r="C205" s="5"/>
+    </row>
+    <row r="206" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A206" s="13" t="s">
+        <v>68</v>
+      </c>
+      <c r="B206" s="13"/>
+      <c r="C206" s="5"/>
+    </row>
+    <row r="207" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A207" s="13"/>
+      <c r="B207" s="13" t="s">
         <v>8</v>
       </c>
-      <c r="C188" s="10" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="189" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A189" s="9"/>
-      <c r="B189" s="9" t="s">
+      <c r="C207" s="5" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="208" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A208" s="13"/>
+      <c r="B208" s="13" t="s">
         <v>10</v>
       </c>
-      <c r="C189" s="10" t="s">
+      <c r="C208" s="5" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="190" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A190" s="9"/>
-      <c r="B190" s="9" t="s">
+    <row r="209" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A209" s="13"/>
+      <c r="B209" s="13" t="s">
         <v>3</v>
       </c>
-      <c r="C190" s="8">
+      <c r="C209" s="7">
         <v>1</v>
       </c>
     </row>
-    <row r="191" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A191" s="9"/>
-      <c r="B191" s="9" t="s">
-        <v>13</v>
-      </c>
-      <c r="C191" s="10"/>
-    </row>
-    <row r="192" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A192" s="9"/>
-      <c r="B192" s="9" t="s">
+    <row r="210" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A210" s="13"/>
+      <c r="B210" s="13" t="s">
         <v>14</v>
       </c>
-      <c r="C192" s="10" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="193" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A193" s="9"/>
-      <c r="B193" s="9" t="s">
+      <c r="C210" s="5" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="211" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A211" s="13"/>
+      <c r="B211" s="13" t="s">
+        <v>52</v>
+      </c>
+      <c r="C211" s="10" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="212" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A212" s="13"/>
+      <c r="B212" s="17" t="s">
         <v>53</v>
       </c>
-      <c r="C193" s="11" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="194" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A194" s="9"/>
-      <c r="B194" s="12" t="s">
-        <v>54</v>
-      </c>
-      <c r="C194" s="13" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="195" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A195" s="9"/>
-      <c r="B195" s="9"/>
-      <c r="C195" s="10"/>
-    </row>
-    <row r="196" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A196" s="9" t="s">
-        <v>67</v>
-      </c>
-      <c r="B196" s="9"/>
-      <c r="C196" s="10"/>
-    </row>
-    <row r="197" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A197" s="9"/>
-      <c r="B197" s="9" t="s">
+      <c r="C212" s="11" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="213" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A213" s="13"/>
+      <c r="B213" s="13"/>
+      <c r="C213" s="5"/>
+    </row>
+    <row r="214" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A214" s="13" t="s">
+        <v>70</v>
+      </c>
+      <c r="B214" s="13"/>
+      <c r="C214" s="5"/>
+    </row>
+    <row r="215" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A215" s="13"/>
+      <c r="B215" s="13" t="s">
         <v>8</v>
       </c>
-      <c r="C197" s="10" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="198" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A198" s="9"/>
-      <c r="B198" s="9" t="s">
+      <c r="C215" s="5" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="216" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A216" s="13"/>
+      <c r="B216" s="13" t="s">
         <v>10</v>
       </c>
-      <c r="C198" s="10" t="s">
+      <c r="C216" s="5" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="199" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A199" s="9"/>
-      <c r="B199" s="9" t="s">
+    <row r="217" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A217" s="13"/>
+      <c r="B217" s="13" t="s">
         <v>3</v>
       </c>
-      <c r="C199" s="8">
+      <c r="C217" s="7">
         <v>1</v>
       </c>
     </row>
-    <row r="200" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A200" s="9"/>
-      <c r="B200" s="9" t="s">
-        <v>13</v>
-      </c>
-      <c r="C200" s="10"/>
-    </row>
-    <row r="201" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A201" s="9"/>
-      <c r="B201" s="9" t="s">
+    <row r="218" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A218" s="13"/>
+      <c r="B218" s="13" t="s">
         <v>14</v>
       </c>
-      <c r="C201" s="10" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="202" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A202" s="9"/>
-      <c r="B202" s="9" t="s">
+      <c r="C218" s="5" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="219" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A219" s="13"/>
+      <c r="B219" s="13" t="s">
+        <v>52</v>
+      </c>
+      <c r="C219" s="10" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="220" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A220" s="13"/>
+      <c r="B220" s="17" t="s">
         <v>53</v>
       </c>
-      <c r="C202" s="14" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="203" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A203" s="9"/>
-      <c r="B203" s="12" t="s">
-        <v>54</v>
-      </c>
-      <c r="C203" s="15" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="204" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A204" s="9"/>
-      <c r="B204" s="9"/>
-      <c r="C204" s="10"/>
-    </row>
-    <row r="205" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A205" s="9" t="s">
-        <v>69</v>
-      </c>
-      <c r="B205" s="9"/>
-      <c r="C205" s="10"/>
-    </row>
-    <row r="206" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A206" s="9"/>
-      <c r="B206" s="9" t="s">
-        <v>8</v>
-      </c>
-      <c r="C206" s="10" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="207" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A207" s="9"/>
-      <c r="B207" s="9" t="s">
-        <v>10</v>
-      </c>
-      <c r="C207" s="10" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="208" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A208" s="9"/>
-      <c r="B208" s="9" t="s">
-        <v>3</v>
-      </c>
-      <c r="C208" s="8">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="209" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A209" s="9"/>
-      <c r="B209" s="9" t="s">
-        <v>13</v>
-      </c>
-      <c r="C209" s="10"/>
-    </row>
-    <row r="210" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A210" s="9"/>
-      <c r="B210" s="9" t="s">
-        <v>14</v>
-      </c>
-      <c r="C210" s="10" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="211" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A211" s="9"/>
-      <c r="B211" s="9" t="s">
-        <v>53</v>
-      </c>
-      <c r="C211" s="14" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="212" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A212" s="9"/>
-      <c r="B212" s="12" t="s">
-        <v>54</v>
-      </c>
-      <c r="C212" s="15" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="213" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A213" s="9"/>
-      <c r="B213" s="9"/>
-      <c r="C213" s="10"/>
-    </row>
-    <row r="214" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A214" s="9" t="s">
-        <v>71</v>
-      </c>
-      <c r="B214" s="9"/>
-      <c r="C214" s="10"/>
-    </row>
-    <row r="215" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A215" s="9"/>
-      <c r="B215" s="9" t="s">
-        <v>8</v>
-      </c>
-      <c r="C215" s="10" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="216" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A216" s="9"/>
-      <c r="B216" s="9" t="s">
-        <v>10</v>
-      </c>
-      <c r="C216" s="10" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="217" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A217" s="9"/>
-      <c r="B217" s="9" t="s">
-        <v>3</v>
-      </c>
-      <c r="C217" s="8">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="218" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A218" s="9"/>
-      <c r="B218" s="9" t="s">
-        <v>13</v>
-      </c>
-      <c r="C218" s="10"/>
-    </row>
-    <row r="219" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A219" s="9"/>
-      <c r="B219" s="9" t="s">
-        <v>14</v>
-      </c>
-      <c r="C219" s="10" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="220" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A220" s="9"/>
-      <c r="B220" s="9" t="s">
-        <v>53</v>
-      </c>
-      <c r="C220" s="14" t="s">
-        <v>75</v>
+      <c r="C220" s="11" t="s">
+        <v>84</v>
       </c>
     </row>
     <row r="221" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A221" s="9"/>
-      <c r="B221" s="12" t="s">
-        <v>54</v>
-      </c>
-      <c r="C221" s="15" t="s">
-        <v>76</v>
-      </c>
+      <c r="C221" s="4"/>
     </row>
     <row r="222" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A222" s="9"/>
-      <c r="B222" s="9"/>
-      <c r="C222" s="10"/>
+      <c r="C222" s="4"/>
     </row>
     <row r="223" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="C223" s="4"/>
@@ -4551,30 +4704,24 @@
     <row r="926" spans="3:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="C926" s="4"/>
     </row>
-    <row r="927" spans="3:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="C927" s="4"/>
-    </row>
-    <row r="928" spans="3:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="C928" s="4"/>
-    </row>
-    <row r="929" spans="3:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="C929" s="4"/>
-    </row>
-    <row r="930" spans="3:3" ht="12" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="931" spans="3:3" ht="12" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="932" spans="3:3" ht="12" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="933" spans="3:3" ht="12" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="934" spans="3:3" ht="12" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="935" spans="3:3" ht="12" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="936" spans="3:3" ht="12" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="937" spans="3:3" ht="12" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="938" spans="3:3" ht="12" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="939" spans="3:3" ht="12" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="940" spans="3:3" ht="12" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="941" spans="3:3" ht="12" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="942" spans="3:3" ht="12" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="943" spans="3:3" ht="12" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="944" spans="3:3" ht="12" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="927" spans="3:3" ht="12" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="928" spans="3:3" ht="12" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="929" ht="12" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="930" ht="12" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="931" ht="12" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="932" ht="12" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="933" ht="12" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="934" ht="12" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="935" ht="12" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="936" ht="12" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="937" ht="12" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="938" ht="12" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="939" ht="12" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="940" ht="12" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="941" ht="12" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="942" ht="12" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="943" ht="12" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="944" ht="12" customHeight="1" x14ac:dyDescent="0.15"/>
     <row r="945" ht="12" customHeight="1" x14ac:dyDescent="0.15"/>
     <row r="946" ht="12" customHeight="1" x14ac:dyDescent="0.15"/>
     <row r="947" ht="12" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -4599,9 +4746,6 @@
     <row r="966" ht="12" customHeight="1" x14ac:dyDescent="0.15"/>
     <row r="967" ht="12" customHeight="1" x14ac:dyDescent="0.15"/>
     <row r="968" ht="12" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="969" ht="12" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="970" ht="12" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="971" ht="12" customHeight="1" x14ac:dyDescent="0.15"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Update buoyancy flux units and definition
</commit_message>
<xml_diff>
--- a/specific_variables/flux-estimates-level1.xlsx
+++ b/specific_variables/flux-estimates-level1.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10510"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10112"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/heather/Desktop/ace-ceda-master/specific_variables/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5A6A1171-56E4-E74C-A0EC-662BB439D8DA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FD7B8075-430D-8943-A3AD-3C17C368362B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="50040" yWindow="-3140" windowWidth="16360" windowHeight="19780" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="18640" windowHeight="19840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="variables-specific" sheetId="2" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="350" uniqueCount="84">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="350" uniqueCount="83">
   <si>
     <t>Variable</t>
   </si>
@@ -106,9 +106,6 @@
     <t>buoyancy_flux</t>
   </si>
   <si>
-    <t>J m-2 s-1</t>
-  </si>
-  <si>
     <t>cell_methods</t>
   </si>
   <si>
@@ -256,9 +253,6 @@
     <t>&lt;derived from file&gt;</t>
   </si>
   <si>
-    <t xml:space="preserve">Buoyancy Flux (&lt;w'Ts'&gt;) </t>
-  </si>
-  <si>
     <t>time: mean</t>
   </si>
   <si>
@@ -272,6 +266,9 @@
   </si>
   <si>
     <t>bad_data good_data _good_for_reasearch suspect_data_good_for_general_use suspect_data_requires_further_checking_but_may_be_ok_for_general_use</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Buoyancy Flux (&lt;w'Ts'&gt;*rho*Cp) </t>
   </si>
 </sst>
 </file>
@@ -347,8 +344,8 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+  <cellXfs count="16">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
@@ -361,25 +358,18 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -413,9 +403,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -453,7 +443,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -559,7 +549,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -701,7 +691,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -714,8 +704,8 @@
   </sheetPr>
   <dimension ref="A1:F967"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A50" workbookViewId="0">
-      <selection activeCell="B80" sqref="B80"/>
+    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="C47" sqref="C47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -750,440 +740,382 @@
       </c>
     </row>
     <row r="2" spans="1:6" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A2" s="10" t="s">
+      <c r="A2" t="s">
         <v>7</v>
       </c>
-      <c r="B2" s="10"/>
-      <c r="C2" s="5"/>
+      <c r="C2" s="4"/>
     </row>
     <row r="3" spans="1:6" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A3" s="10"/>
-      <c r="B3" s="10" t="s">
+      <c r="B3" t="s">
         <v>8</v>
       </c>
-      <c r="C3" s="5" t="s">
+      <c r="C3" s="4" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="4" spans="1:6" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A4" s="10"/>
-      <c r="B4" s="10" t="s">
+      <c r="B4" t="s">
         <v>10</v>
       </c>
-      <c r="C4" s="5" t="s">
+      <c r="C4" s="4" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="5" spans="1:6" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A5" s="10"/>
-      <c r="B5" s="10" t="s">
+      <c r="B5" t="s">
         <v>3</v>
       </c>
-      <c r="C5" s="5" t="s">
+      <c r="C5" s="4" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="6" spans="1:6" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A6" s="10"/>
-      <c r="B6" s="10" t="s">
+      <c r="B6" t="s">
         <v>14</v>
       </c>
-      <c r="C6" s="5" t="s">
+      <c r="C6" s="4" t="s">
         <v>15</v>
       </c>
       <c r="D6" s="4"/>
     </row>
     <row r="7" spans="1:6" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A7" s="10"/>
-      <c r="B7" s="10" t="s">
+      <c r="B7" t="s">
         <v>16</v>
       </c>
-      <c r="C7" s="13">
+      <c r="C7" s="5">
         <v>-1E+20</v>
       </c>
     </row>
     <row r="8" spans="1:6" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A8" s="10"/>
-      <c r="B8" s="10" t="s">
+      <c r="B8" t="s">
         <v>17</v>
       </c>
-      <c r="C8" s="12" t="s">
+      <c r="C8" s="10" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" ht="12" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B9" t="s">
+        <v>18</v>
+      </c>
+      <c r="C9" s="10" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" ht="12" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B10" t="s">
+        <v>19</v>
+      </c>
+      <c r="C10" s="4" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" ht="12" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="C11" s="4"/>
+    </row>
+    <row r="12" spans="1:6" ht="12" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A12" t="s">
+        <v>21</v>
+      </c>
+      <c r="C12" s="4"/>
+    </row>
+    <row r="13" spans="1:6" ht="12" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B13" t="s">
+        <v>8</v>
+      </c>
+      <c r="C13" s="4" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" ht="12" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B14" t="s">
+        <v>10</v>
+      </c>
+      <c r="C14" s="4" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" ht="12" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B15" t="s">
+        <v>3</v>
+      </c>
+      <c r="C15" s="10" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" ht="12" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B16" t="s">
+        <v>14</v>
+      </c>
+      <c r="C16" s="4" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" ht="12" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B17" t="s">
+        <v>16</v>
+      </c>
+      <c r="C17" s="5">
+        <v>-1E+20</v>
+      </c>
+      <c r="D17" s="4"/>
+    </row>
+    <row r="18" spans="1:4" ht="12" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B18" t="s">
+        <v>17</v>
+      </c>
+      <c r="C18" s="6" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" ht="12" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B19" t="s">
+        <v>18</v>
+      </c>
+      <c r="C19" s="6" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" ht="12" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B20" t="s">
+        <v>19</v>
+      </c>
+      <c r="C20" s="4" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" ht="12" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="22" spans="1:4" ht="12" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A22" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" ht="12" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B23" t="s">
+        <v>8</v>
+      </c>
+      <c r="C23" s="9" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" ht="12" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B24" t="s">
+        <v>10</v>
+      </c>
+      <c r="C24" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" ht="12" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B25" t="s">
+        <v>3</v>
+      </c>
+      <c r="C25" s="10" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" ht="12" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B26" t="s">
+        <v>14</v>
+      </c>
+      <c r="C26" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" ht="12" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B27" t="s">
+        <v>16</v>
+      </c>
+      <c r="C27" s="5">
+        <v>-1E+20</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" ht="12" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B28" t="s">
+        <v>17</v>
+      </c>
+      <c r="C28" s="6" t="s">
+        <v>76</v>
+      </c>
+      <c r="D28" s="4"/>
+    </row>
+    <row r="29" spans="1:4" ht="12" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B29" t="s">
+        <v>18</v>
+      </c>
+      <c r="C29" s="6" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" ht="12" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B30" t="s">
+        <v>28</v>
+      </c>
+      <c r="C30" s="13" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="9" spans="1:6" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A9" s="10"/>
-      <c r="B9" s="10" t="s">
+    <row r="31" spans="1:4" ht="12" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B31" t="s">
+        <v>19</v>
+      </c>
+      <c r="C31" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" ht="12" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="C32" s="4"/>
+    </row>
+    <row r="33" spans="1:4" ht="12" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A33" t="s">
+        <v>25</v>
+      </c>
+      <c r="C33" s="4"/>
+    </row>
+    <row r="34" spans="1:4" ht="12" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B34" t="s">
+        <v>8</v>
+      </c>
+      <c r="C34" s="4" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" ht="12" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B35" t="s">
+        <v>10</v>
+      </c>
+      <c r="C35" s="4" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" ht="12" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B36" t="s">
+        <v>3</v>
+      </c>
+      <c r="C36" s="10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" ht="12" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B37" t="s">
+        <v>14</v>
+      </c>
+      <c r="C37" s="4" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" ht="12" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B38" t="s">
+        <v>16</v>
+      </c>
+      <c r="C38" s="5">
+        <v>-1E+20</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" ht="12" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B39" t="s">
+        <v>17</v>
+      </c>
+      <c r="C39" s="6" t="s">
+        <v>76</v>
+      </c>
+      <c r="D39" s="4"/>
+    </row>
+    <row r="40" spans="1:4" ht="12" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B40" t="s">
         <v>18</v>
       </c>
-      <c r="C9" s="12" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A10" s="10"/>
-      <c r="B10" s="10" t="s">
+      <c r="C40" s="6" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" ht="12" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B41" t="s">
         <v>19</v>
       </c>
-      <c r="C10" s="5" t="s">
+      <c r="C41" s="4" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="11" spans="1:6" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A11" s="10"/>
-      <c r="B11" s="10"/>
-      <c r="C11" s="5"/>
-    </row>
-    <row r="12" spans="1:6" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A12" s="10" t="s">
-        <v>21</v>
-      </c>
-      <c r="B12" s="10"/>
-      <c r="C12" s="5"/>
-    </row>
-    <row r="13" spans="1:6" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A13" s="10"/>
-      <c r="B13" s="10" t="s">
+    <row r="42" spans="1:4" ht="12" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="C42" s="4"/>
+    </row>
+    <row r="43" spans="1:4" ht="12" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A43" t="s">
+        <v>27</v>
+      </c>
+      <c r="C43" s="4"/>
+    </row>
+    <row r="44" spans="1:4" ht="12" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B44" t="s">
         <v>8</v>
       </c>
-      <c r="C13" s="5" t="s">
+      <c r="C44" s="4" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="14" spans="1:6" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A14" s="10"/>
-      <c r="B14" s="10" t="s">
+    <row r="45" spans="1:4" ht="12" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B45" t="s">
         <v>10</v>
       </c>
-      <c r="C14" s="5" t="s">
+      <c r="C45" s="4" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="15" spans="1:6" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A15" s="10"/>
-      <c r="B15" s="10" t="s">
+    <row r="46" spans="1:4" ht="12" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B46" t="s">
         <v>3</v>
       </c>
-      <c r="C15" s="12" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A16" s="10"/>
-      <c r="B16" s="10" t="s">
+      <c r="C46" s="4" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4" ht="12" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B47" t="s">
         <v>14</v>
       </c>
-      <c r="C16" s="5" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A17" s="10"/>
-      <c r="B17" s="10" t="s">
+      <c r="C47" s="11" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4" ht="12" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B48" t="s">
         <v>16</v>
       </c>
-      <c r="C17" s="13">
+      <c r="C48" s="5">
         <v>-1E+20</v>
       </c>
-      <c r="D17" s="4"/>
-    </row>
-    <row r="18" spans="1:4" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A18" s="10"/>
-      <c r="B18" s="10" t="s">
+    </row>
+    <row r="49" spans="1:4" ht="12" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B49" t="s">
         <v>17</v>
       </c>
-      <c r="C18" s="7" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A19" s="10"/>
-      <c r="B19" s="10" t="s">
+      <c r="C49" s="6" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4" ht="12" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B50" t="s">
         <v>18</v>
       </c>
-      <c r="C19" s="7" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A20" s="10"/>
-      <c r="B20" s="10" t="s">
+      <c r="C50" s="6" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4" ht="12" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B51" t="s">
+        <v>28</v>
+      </c>
+      <c r="C51" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="D51" s="4"/>
+    </row>
+    <row r="52" spans="1:4" ht="12" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B52" t="s">
         <v>19</v>
       </c>
-      <c r="C20" s="5" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A21" s="10"/>
-      <c r="B21" s="10"/>
-      <c r="C21" s="10"/>
-    </row>
-    <row r="22" spans="1:4" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A22" s="10" t="s">
-        <v>74</v>
-      </c>
-      <c r="B22" s="10"/>
-      <c r="C22" s="10"/>
-    </row>
-    <row r="23" spans="1:4" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A23" s="10"/>
-      <c r="B23" s="10" t="s">
-        <v>8</v>
-      </c>
-      <c r="C23" s="11" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A24" s="10"/>
-      <c r="B24" s="10" t="s">
-        <v>10</v>
-      </c>
-      <c r="C24" s="10" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="25" spans="1:4" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A25" s="10"/>
-      <c r="B25" s="10" t="s">
-        <v>3</v>
-      </c>
-      <c r="C25" s="12" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="26" spans="1:4" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A26" s="10"/>
-      <c r="B26" s="10" t="s">
-        <v>14</v>
-      </c>
-      <c r="C26" s="10" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="27" spans="1:4" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A27" s="10"/>
-      <c r="B27" s="10" t="s">
-        <v>16</v>
-      </c>
-      <c r="C27" s="13">
-        <v>-1E+20</v>
-      </c>
-    </row>
-    <row r="28" spans="1:4" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A28" s="10"/>
-      <c r="B28" s="10" t="s">
-        <v>17</v>
-      </c>
-      <c r="C28" s="7" t="s">
-        <v>77</v>
-      </c>
-      <c r="D28" s="4"/>
-    </row>
-    <row r="29" spans="1:4" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A29" s="10"/>
-      <c r="B29" s="10" t="s">
-        <v>18</v>
-      </c>
-      <c r="C29" s="7" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="30" spans="1:4" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A30" s="10"/>
-      <c r="B30" s="10" t="s">
-        <v>29</v>
-      </c>
-      <c r="C30" s="16" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="31" spans="1:4" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A31" s="10"/>
-      <c r="B31" s="10" t="s">
-        <v>19</v>
-      </c>
-      <c r="C31" s="10" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="32" spans="1:4" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A32" s="10"/>
-      <c r="B32" s="10"/>
-      <c r="C32" s="5"/>
-    </row>
-    <row r="33" spans="1:4" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A33" s="10" t="s">
-        <v>25</v>
-      </c>
-      <c r="B33" s="10"/>
-      <c r="C33" s="5"/>
-    </row>
-    <row r="34" spans="1:4" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A34" s="10"/>
-      <c r="B34" s="10" t="s">
-        <v>8</v>
-      </c>
-      <c r="C34" s="5" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="35" spans="1:4" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A35" s="10"/>
-      <c r="B35" s="10" t="s">
-        <v>10</v>
-      </c>
-      <c r="C35" s="5" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="36" spans="1:4" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A36" s="10"/>
-      <c r="B36" s="10" t="s">
-        <v>3</v>
-      </c>
-      <c r="C36" s="12">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="37" spans="1:4" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A37" s="10"/>
-      <c r="B37" s="10" t="s">
-        <v>14</v>
-      </c>
-      <c r="C37" s="5" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="38" spans="1:4" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A38" s="10"/>
-      <c r="B38" s="10" t="s">
-        <v>16</v>
-      </c>
-      <c r="C38" s="13">
-        <v>-1E+20</v>
-      </c>
-    </row>
-    <row r="39" spans="1:4" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A39" s="10"/>
-      <c r="B39" s="10" t="s">
-        <v>17</v>
-      </c>
-      <c r="C39" s="7" t="s">
-        <v>77</v>
-      </c>
-      <c r="D39" s="4"/>
-    </row>
-    <row r="40" spans="1:4" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A40" s="10"/>
-      <c r="B40" s="10" t="s">
-        <v>18</v>
-      </c>
-      <c r="C40" s="7" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="41" spans="1:4" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A41" s="10"/>
-      <c r="B41" s="10" t="s">
-        <v>19</v>
-      </c>
-      <c r="C41" s="5" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="42" spans="1:4" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A42" s="10"/>
-      <c r="B42" s="10"/>
-      <c r="C42" s="5"/>
-    </row>
-    <row r="43" spans="1:4" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A43" s="10" t="s">
-        <v>27</v>
-      </c>
-      <c r="B43" s="10"/>
-      <c r="C43" s="5"/>
-    </row>
-    <row r="44" spans="1:4" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A44" s="10"/>
-      <c r="B44" s="10" t="s">
-        <v>8</v>
-      </c>
-      <c r="C44" s="5" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="45" spans="1:4" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A45" s="10"/>
-      <c r="B45" s="10" t="s">
-        <v>10</v>
-      </c>
-      <c r="C45" s="5" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="46" spans="1:4" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A46" s="10"/>
-      <c r="B46" s="10" t="s">
-        <v>3</v>
-      </c>
-      <c r="C46" s="5" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="47" spans="1:4" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A47" s="10"/>
-      <c r="B47" s="10" t="s">
-        <v>14</v>
-      </c>
-      <c r="C47" s="14" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="48" spans="1:4" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A48" s="10"/>
-      <c r="B48" s="10" t="s">
-        <v>16</v>
-      </c>
-      <c r="C48" s="13">
-        <v>-1E+20</v>
-      </c>
-    </row>
-    <row r="49" spans="1:4" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A49" s="10"/>
-      <c r="B49" s="10" t="s">
-        <v>17</v>
-      </c>
-      <c r="C49" s="7" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="50" spans="1:4" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A50" s="10"/>
-      <c r="B50" s="10" t="s">
-        <v>18</v>
-      </c>
-      <c r="C50" s="7" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="51" spans="1:4" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A51" s="10"/>
-      <c r="B51" s="10" t="s">
-        <v>29</v>
-      </c>
-      <c r="C51" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="D51" s="4"/>
-    </row>
-    <row r="52" spans="1:4" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A52" s="10"/>
-      <c r="B52" s="10" t="s">
-        <v>19</v>
-      </c>
-      <c r="C52" s="5" t="s">
+      <c r="C52" s="4" t="s">
         <v>20</v>
       </c>
     </row>
@@ -1192,7 +1124,7 @@
     </row>
     <row r="54" spans="1:4" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A54" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C54" s="4"/>
     </row>
@@ -1200,7 +1132,7 @@
       <c r="B55" t="s">
         <v>8</v>
       </c>
-      <c r="C55" s="5" t="s">
+      <c r="C55" s="4" t="s">
         <v>22</v>
       </c>
     </row>
@@ -1217,7 +1149,7 @@
         <v>3</v>
       </c>
       <c r="C57" s="4" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="58" spans="1:4" ht="12" customHeight="1" x14ac:dyDescent="0.15">
@@ -1225,42 +1157,40 @@
         <v>14</v>
       </c>
       <c r="C58" s="4" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="59" spans="1:4" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B59" t="s">
         <v>16</v>
       </c>
-      <c r="C59" s="6">
+      <c r="C59" s="5">
         <v>-1E+20</v>
       </c>
     </row>
     <row r="60" spans="1:4" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A60" s="10"/>
-      <c r="B60" s="10" t="s">
+      <c r="B60" t="s">
         <v>17</v>
       </c>
-      <c r="C60" s="7" t="s">
-        <v>77</v>
+      <c r="C60" s="6" t="s">
+        <v>76</v>
       </c>
     </row>
     <row r="61" spans="1:4" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A61" s="10"/>
-      <c r="B61" s="10" t="s">
+      <c r="B61" t="s">
         <v>18</v>
       </c>
-      <c r="C61" s="7" t="s">
-        <v>77</v>
+      <c r="C61" s="6" t="s">
+        <v>76</v>
       </c>
       <c r="D61" s="4"/>
     </row>
     <row r="62" spans="1:4" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B62" t="s">
+        <v>28</v>
+      </c>
+      <c r="C62" s="4" t="s">
         <v>29</v>
-      </c>
-      <c r="C62" s="4" t="s">
-        <v>30</v>
       </c>
     </row>
     <row r="63" spans="1:4" ht="12" customHeight="1" x14ac:dyDescent="0.15">
@@ -1275,295 +1205,259 @@
       <c r="C64" s="4"/>
     </row>
     <row r="65" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A65" s="10" t="s">
+      <c r="A65" t="s">
+        <v>33</v>
+      </c>
+      <c r="C65" s="4"/>
+    </row>
+    <row r="66" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B66" t="s">
+        <v>8</v>
+      </c>
+      <c r="C66" s="4" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="67" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B67" t="s">
+        <v>10</v>
+      </c>
+      <c r="C67" s="4" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="68" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B68" t="s">
+        <v>3</v>
+      </c>
+      <c r="C68" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="B65" s="10"/>
-      <c r="C65" s="5"/>
-    </row>
-    <row r="66" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A66" s="10"/>
-      <c r="B66" s="10" t="s">
+    </row>
+    <row r="69" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B69" t="s">
+        <v>14</v>
+      </c>
+      <c r="C69" s="4" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="70" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B70" t="s">
+        <v>16</v>
+      </c>
+      <c r="C70" s="5">
+        <v>-1E+20</v>
+      </c>
+    </row>
+    <row r="71" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B71" t="s">
+        <v>17</v>
+      </c>
+      <c r="C71" s="6" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="72" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B72" t="s">
+        <v>18</v>
+      </c>
+      <c r="C72" s="6" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="73" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B73" t="s">
+        <v>28</v>
+      </c>
+      <c r="C73" s="4" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="74" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B74" t="s">
+        <v>19</v>
+      </c>
+      <c r="C74" s="4" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="75" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="C75" s="4"/>
+    </row>
+    <row r="76" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A76" t="s">
+        <v>36</v>
+      </c>
+      <c r="C76" s="4"/>
+    </row>
+    <row r="77" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B77" t="s">
         <v>8</v>
       </c>
-      <c r="C66" s="5" t="s">
+      <c r="C77" s="4" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="67" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A67" s="10"/>
-      <c r="B67" s="10" t="s">
+    <row r="78" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B78" t="s">
         <v>10</v>
       </c>
-      <c r="C67" s="5" t="s">
+      <c r="C78" s="4" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="68" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A68" s="10"/>
-      <c r="B68" s="10" t="s">
+    <row r="79" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B79" t="s">
         <v>3</v>
       </c>
-      <c r="C68" s="5" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="69" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A69" s="10"/>
-      <c r="B69" s="10" t="s">
+      <c r="C79" s="4" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="80" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B80" t="s">
+        <v>13</v>
+      </c>
+      <c r="C80" s="4" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="81" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B81" t="s">
         <v>14</v>
       </c>
-      <c r="C69" s="5" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="70" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A70" s="10"/>
-      <c r="B70" s="10" t="s">
+      <c r="C81" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="82" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B82" t="s">
         <v>16</v>
       </c>
-      <c r="C70" s="13">
+      <c r="C82" s="5">
         <v>-1E+20</v>
       </c>
     </row>
-    <row r="71" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A71" s="10"/>
-      <c r="B71" s="10" t="s">
+    <row r="83" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B83" t="s">
         <v>17</v>
       </c>
-      <c r="C71" s="7" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="72" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A72" s="10"/>
-      <c r="B72" s="10" t="s">
+      <c r="C83" s="6" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="84" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B84" t="s">
         <v>18</v>
       </c>
-      <c r="C72" s="7" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="73" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A73" s="10"/>
-      <c r="B73" s="10" t="s">
+      <c r="C84" s="6" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="85" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B85" t="s">
+        <v>28</v>
+      </c>
+      <c r="C85" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="C73" s="5" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="74" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A74" s="10"/>
-      <c r="B74" s="10" t="s">
+    </row>
+    <row r="86" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B86" t="s">
         <v>19</v>
       </c>
-      <c r="C74" s="5" t="s">
+      <c r="C86" s="4" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="75" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A75" s="10"/>
-      <c r="B75" s="10"/>
-      <c r="C75" s="5"/>
-    </row>
-    <row r="76" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A76" s="10" t="s">
+    <row r="87" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="C87" s="4"/>
+    </row>
+    <row r="88" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A88" t="s">
+        <v>39</v>
+      </c>
+      <c r="C88" s="4"/>
+    </row>
+    <row r="89" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B89" t="s">
+        <v>8</v>
+      </c>
+      <c r="C89" s="4" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="90" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B90" t="s">
+        <v>10</v>
+      </c>
+      <c r="C90" s="4" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="91" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B91" t="s">
+        <v>3</v>
+      </c>
+      <c r="C91" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="B76" s="10"/>
-      <c r="C76" s="5"/>
-    </row>
-    <row r="77" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A77" s="10"/>
-      <c r="B77" s="10" t="s">
-        <v>8</v>
-      </c>
-      <c r="C77" s="5" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="78" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A78" s="10"/>
-      <c r="B78" s="10" t="s">
-        <v>10</v>
-      </c>
-      <c r="C78" s="5" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="79" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A79" s="10"/>
-      <c r="B79" s="10" t="s">
-        <v>3</v>
-      </c>
-      <c r="C79" s="5" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="80" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A80" s="10"/>
-      <c r="B80" s="10" t="s">
+    </row>
+    <row r="92" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B92" t="s">
         <v>13</v>
       </c>
-      <c r="C80" s="5" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="81" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A81" s="10"/>
-      <c r="B81" s="10" t="s">
+      <c r="C92" s="4" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="93" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B93" t="s">
         <v>14</v>
       </c>
-      <c r="C81" s="5" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="82" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A82" s="10"/>
-      <c r="B82" s="10" t="s">
+      <c r="C93" s="4" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="94" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B94" t="s">
         <v>16</v>
       </c>
-      <c r="C82" s="13">
+      <c r="C94" s="5">
         <v>-1E+20</v>
       </c>
     </row>
-    <row r="83" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A83" s="10"/>
-      <c r="B83" s="10" t="s">
+    <row r="95" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B95" t="s">
         <v>17</v>
       </c>
-      <c r="C83" s="7" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="84" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A84" s="10"/>
-      <c r="B84" s="10" t="s">
+      <c r="C95" s="6" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="96" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B96" t="s">
         <v>18</v>
       </c>
-      <c r="C84" s="7" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="85" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A85" s="10"/>
-      <c r="B85" s="10" t="s">
+      <c r="C96" s="6" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="97" spans="1:4" ht="12" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B97" t="s">
+        <v>28</v>
+      </c>
+      <c r="C97" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="C85" s="5" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="86" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A86" s="10"/>
-      <c r="B86" s="10" t="s">
+      <c r="D97" s="4"/>
+    </row>
+    <row r="98" spans="1:4" ht="12" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B98" t="s">
         <v>19</v>
       </c>
-      <c r="C86" s="5" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="87" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A87" s="10"/>
-      <c r="B87" s="10"/>
-      <c r="C87" s="5"/>
-    </row>
-    <row r="88" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A88" s="10" t="s">
-        <v>40</v>
-      </c>
-      <c r="B88" s="10"/>
-      <c r="C88" s="5"/>
-    </row>
-    <row r="89" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A89" s="10"/>
-      <c r="B89" s="10" t="s">
-        <v>8</v>
-      </c>
-      <c r="C89" s="5" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="90" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A90" s="10"/>
-      <c r="B90" s="10" t="s">
-        <v>10</v>
-      </c>
-      <c r="C90" s="5" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="91" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A91" s="10"/>
-      <c r="B91" s="10" t="s">
-        <v>3</v>
-      </c>
-      <c r="C91" s="5" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="92" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A92" s="10"/>
-      <c r="B92" s="10" t="s">
-        <v>13</v>
-      </c>
-      <c r="C92" s="5" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="93" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A93" s="10"/>
-      <c r="B93" s="10" t="s">
-        <v>14</v>
-      </c>
-      <c r="C93" s="5" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="94" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A94" s="10"/>
-      <c r="B94" s="10" t="s">
-        <v>16</v>
-      </c>
-      <c r="C94" s="13">
-        <v>-1E+20</v>
-      </c>
-    </row>
-    <row r="95" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A95" s="10"/>
-      <c r="B95" s="10" t="s">
-        <v>17</v>
-      </c>
-      <c r="C95" s="7" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="96" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A96" s="10"/>
-      <c r="B96" s="10" t="s">
-        <v>18</v>
-      </c>
-      <c r="C96" s="7" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="97" spans="1:4" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A97" s="10"/>
-      <c r="B97" s="10" t="s">
-        <v>29</v>
-      </c>
-      <c r="C97" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="D97" s="4"/>
-    </row>
-    <row r="98" spans="1:4" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A98" s="10"/>
-      <c r="B98" s="10" t="s">
-        <v>19</v>
-      </c>
-      <c r="C98" s="5" t="s">
+      <c r="C98" s="4" t="s">
         <v>20</v>
       </c>
     </row>
@@ -1571,276 +1465,244 @@
       <c r="C99" s="4"/>
     </row>
     <row r="100" spans="1:4" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A100" s="10" t="s">
+      <c r="A100" t="s">
+        <v>41</v>
+      </c>
+      <c r="C100" s="4"/>
+    </row>
+    <row r="101" spans="1:4" ht="12" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B101" t="s">
+        <v>8</v>
+      </c>
+      <c r="C101" s="4" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="102" spans="1:4" ht="12" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B102" t="s">
+        <v>10</v>
+      </c>
+      <c r="C102" s="4" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="103" spans="1:4" ht="12" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B103" t="s">
+        <v>3</v>
+      </c>
+      <c r="C103" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="B100" s="10"/>
-      <c r="C100" s="5"/>
-    </row>
-    <row r="101" spans="1:4" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A101" s="10"/>
-      <c r="B101" s="10" t="s">
+    </row>
+    <row r="104" spans="1:4" ht="12" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B104" t="s">
+        <v>14</v>
+      </c>
+      <c r="C104" s="4" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="105" spans="1:4" ht="12" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B105" t="s">
+        <v>16</v>
+      </c>
+      <c r="C105" s="5">
+        <v>-1E+20</v>
+      </c>
+    </row>
+    <row r="106" spans="1:4" ht="12" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B106" t="s">
+        <v>17</v>
+      </c>
+      <c r="C106" s="6" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="107" spans="1:4" ht="12" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B107" t="s">
+        <v>18</v>
+      </c>
+      <c r="C107" s="6" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="108" spans="1:4" ht="12" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B108" t="s">
+        <v>28</v>
+      </c>
+      <c r="C108" s="4" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="109" spans="1:4" ht="12" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B109" t="s">
+        <v>19</v>
+      </c>
+      <c r="C109" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="D109" s="4"/>
+    </row>
+    <row r="110" spans="1:4" ht="12" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="C110" s="4"/>
+    </row>
+    <row r="111" spans="1:4" ht="12" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A111" t="s">
+        <v>44</v>
+      </c>
+      <c r="C111" s="4"/>
+    </row>
+    <row r="112" spans="1:4" ht="12" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B112" t="s">
         <v>8</v>
       </c>
-      <c r="C101" s="5" t="s">
+      <c r="C112" s="4" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="102" spans="1:4" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A102" s="10"/>
-      <c r="B102" s="10" t="s">
+    <row r="113" spans="1:4" ht="12" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B113" t="s">
         <v>10</v>
       </c>
-      <c r="C102" s="5" t="s">
+      <c r="C113" s="4" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="103" spans="1:4" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A103" s="10"/>
-      <c r="B103" s="10" t="s">
+    <row r="114" spans="1:4" ht="12" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B114" t="s">
         <v>3</v>
       </c>
-      <c r="C103" s="5" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="104" spans="1:4" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A104" s="10"/>
-      <c r="B104" s="10" t="s">
+      <c r="C114" s="4" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="115" spans="1:4" ht="12" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B115" t="s">
         <v>14</v>
       </c>
-      <c r="C104" s="5" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="105" spans="1:4" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A105" s="10"/>
-      <c r="B105" s="10" t="s">
+      <c r="C115" s="4" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="116" spans="1:4" ht="12" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B116" t="s">
         <v>16</v>
       </c>
-      <c r="C105" s="13">
+      <c r="C116" s="5">
         <v>-1E+20</v>
       </c>
     </row>
-    <row r="106" spans="1:4" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A106" s="10"/>
-      <c r="B106" s="10" t="s">
+    <row r="117" spans="1:4" ht="12" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B117" t="s">
         <v>17</v>
       </c>
-      <c r="C106" s="7" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="107" spans="1:4" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A107" s="10"/>
-      <c r="B107" s="10" t="s">
+      <c r="C117" s="6" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="118" spans="1:4" ht="12" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B118" t="s">
         <v>18</v>
       </c>
-      <c r="C107" s="7" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="108" spans="1:4" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A108" s="10"/>
-      <c r="B108" s="10" t="s">
+      <c r="C118" s="6" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="119" spans="1:4" ht="12" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B119" t="s">
+        <v>28</v>
+      </c>
+      <c r="C119" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="C108" s="5" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="109" spans="1:4" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A109" s="10"/>
-      <c r="B109" s="10" t="s">
+    </row>
+    <row r="120" spans="1:4" ht="12" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B120" t="s">
         <v>19</v>
       </c>
-      <c r="C109" s="5" t="s">
+      <c r="C120" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="D109" s="4"/>
-    </row>
-    <row r="110" spans="1:4" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A110" s="10"/>
-      <c r="B110" s="10"/>
-      <c r="C110" s="5"/>
-    </row>
-    <row r="111" spans="1:4" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A111" s="10" t="s">
-        <v>45</v>
-      </c>
-      <c r="B111" s="10"/>
-      <c r="C111" s="5"/>
-    </row>
-    <row r="112" spans="1:4" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A112" s="10"/>
-      <c r="B112" s="10" t="s">
+    </row>
+    <row r="121" spans="1:4" ht="12" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="C121" s="4"/>
+      <c r="D121" s="4"/>
+    </row>
+    <row r="122" spans="1:4" ht="12" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A122" t="s">
+        <v>46</v>
+      </c>
+      <c r="C122" s="4"/>
+    </row>
+    <row r="123" spans="1:4" ht="12" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B123" t="s">
         <v>8</v>
       </c>
-      <c r="C112" s="5" t="s">
+      <c r="C123" s="4" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="113" spans="1:4" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A113" s="10"/>
-      <c r="B113" s="10" t="s">
+    <row r="124" spans="1:4" ht="12" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B124" t="s">
         <v>10</v>
       </c>
-      <c r="C113" s="5" t="s">
+      <c r="C124" s="4" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="114" spans="1:4" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A114" s="10"/>
-      <c r="B114" s="10" t="s">
+    <row r="125" spans="1:4" ht="12" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B125" t="s">
         <v>3</v>
       </c>
-      <c r="C114" s="5" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="115" spans="1:4" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A115" s="10"/>
-      <c r="B115" s="10" t="s">
+      <c r="C125" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="126" spans="1:4" ht="12" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B126" t="s">
         <v>14</v>
       </c>
-      <c r="C115" s="5" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="116" spans="1:4" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A116" s="10"/>
-      <c r="B116" s="10" t="s">
+      <c r="C126" s="4" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="127" spans="1:4" ht="12" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B127" t="s">
         <v>16</v>
       </c>
-      <c r="C116" s="13">
+      <c r="C127" s="5">
         <v>-1E+20</v>
       </c>
     </row>
-    <row r="117" spans="1:4" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A117" s="10"/>
-      <c r="B117" s="10" t="s">
+    <row r="128" spans="1:4" ht="12" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B128" t="s">
         <v>17</v>
       </c>
-      <c r="C117" s="7" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="118" spans="1:4" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A118" s="10"/>
-      <c r="B118" s="10" t="s">
+      <c r="C128" s="6" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="129" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B129" t="s">
         <v>18</v>
       </c>
-      <c r="C118" s="7" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="119" spans="1:4" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A119" s="10"/>
-      <c r="B119" s="10" t="s">
+      <c r="C129" s="6" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="130" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B130" t="s">
+        <v>28</v>
+      </c>
+      <c r="C130" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="C119" s="5" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="120" spans="1:4" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A120" s="10"/>
-      <c r="B120" s="10" t="s">
+    </row>
+    <row r="131" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B131" t="s">
         <v>19</v>
       </c>
-      <c r="C120" s="5" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="121" spans="1:4" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="C121" s="5"/>
-      <c r="D121" s="4"/>
-    </row>
-    <row r="122" spans="1:4" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A122" s="10" t="s">
-        <v>47</v>
-      </c>
-      <c r="B122" s="10"/>
-      <c r="C122" s="5"/>
-    </row>
-    <row r="123" spans="1:4" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A123" s="10"/>
-      <c r="B123" s="10" t="s">
-        <v>8</v>
-      </c>
-      <c r="C123" s="5" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="124" spans="1:4" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A124" s="10"/>
-      <c r="B124" s="10" t="s">
-        <v>10</v>
-      </c>
-      <c r="C124" s="5" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="125" spans="1:4" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A125" s="10"/>
-      <c r="B125" s="10" t="s">
-        <v>3</v>
-      </c>
-      <c r="C125" s="5">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="126" spans="1:4" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A126" s="10"/>
-      <c r="B126" s="10" t="s">
-        <v>14</v>
-      </c>
-      <c r="C126" s="5" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="127" spans="1:4" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A127" s="10"/>
-      <c r="B127" s="10" t="s">
-        <v>16</v>
-      </c>
-      <c r="C127" s="13">
-        <v>-1E+20</v>
-      </c>
-    </row>
-    <row r="128" spans="1:4" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A128" s="10"/>
-      <c r="B128" s="10" t="s">
-        <v>17</v>
-      </c>
-      <c r="C128" s="7" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="129" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A129" s="10"/>
-      <c r="B129" s="10" t="s">
-        <v>18</v>
-      </c>
-      <c r="C129" s="7" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="130" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A130" s="10"/>
-      <c r="B130" s="10" t="s">
-        <v>29</v>
-      </c>
-      <c r="C130" s="5" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="131" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A131" s="10"/>
-      <c r="B131" s="10" t="s">
-        <v>19</v>
-      </c>
-      <c r="C131" s="5" t="s">
+      <c r="C131" s="4" t="s">
         <v>20</v>
       </c>
     </row>
@@ -1848,724 +1710,724 @@
       <c r="C132" s="4"/>
     </row>
     <row r="133" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A133" s="11" t="s">
+      <c r="A133" s="9" t="s">
+        <v>48</v>
+      </c>
+      <c r="B133" s="9"/>
+      <c r="C133" s="4"/>
+    </row>
+    <row r="134" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A134" s="9"/>
+      <c r="B134" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="C134" s="4" t="s">
         <v>49</v>
       </c>
-      <c r="B133" s="11"/>
-      <c r="C133" s="5"/>
-    </row>
-    <row r="134" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A134" s="11"/>
-      <c r="B134" s="11" t="s">
+    </row>
+    <row r="135" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A135" s="9"/>
+      <c r="B135" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="C135" s="4" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="136" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A136" s="9"/>
+      <c r="B136" s="9" t="s">
+        <v>3</v>
+      </c>
+      <c r="C136" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="137" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A137" s="9"/>
+      <c r="B137" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="C137" s="4" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="138" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A138" s="9"/>
+      <c r="B138" s="9" t="s">
+        <v>51</v>
+      </c>
+      <c r="C138" s="14" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="139" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A139" s="9"/>
+      <c r="B139" s="12" t="s">
+        <v>52</v>
+      </c>
+      <c r="C139" s="15" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="140" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A140" s="9"/>
+      <c r="B140" s="9"/>
+      <c r="C140" s="4"/>
+    </row>
+    <row r="141" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A141" s="9" t="s">
+        <v>53</v>
+      </c>
+      <c r="B141" s="9"/>
+      <c r="C141" s="4"/>
+    </row>
+    <row r="142" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A142" s="9"/>
+      <c r="B142" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="C134" s="5" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="135" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A135" s="11"/>
-      <c r="B135" s="11" t="s">
+      <c r="C142" s="4" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="143" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A143" s="9"/>
+      <c r="B143" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="C135" s="5" t="s">
+      <c r="C143" s="4" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="136" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A136" s="11"/>
-      <c r="B136" s="11" t="s">
+    <row r="144" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A144" s="9"/>
+      <c r="B144" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="C136" s="7">
+      <c r="C144" s="6">
         <v>1</v>
       </c>
     </row>
-    <row r="137" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A137" s="11"/>
-      <c r="B137" s="11" t="s">
+    <row r="145" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A145" s="9"/>
+      <c r="B145" s="9" t="s">
         <v>14</v>
       </c>
-      <c r="C137" s="5" t="s">
+      <c r="C145" s="4" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="146" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A146" s="9"/>
+      <c r="B146" s="9" t="s">
         <v>51</v>
       </c>
-    </row>
-    <row r="138" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A138" s="11"/>
-      <c r="B138" s="11" t="s">
+      <c r="C146" s="14" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="147" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A147" s="9"/>
+      <c r="B147" s="12" t="s">
         <v>52</v>
       </c>
-      <c r="C138" s="17" t="s">
+      <c r="C147" s="15" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="148" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A148" s="9"/>
+      <c r="B148" s="9"/>
+      <c r="C148" s="4"/>
+    </row>
+    <row r="149" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A149" s="9" t="s">
+        <v>55</v>
+      </c>
+      <c r="B149" s="9"/>
+      <c r="C149" s="4"/>
+    </row>
+    <row r="150" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A150" s="9"/>
+      <c r="B150" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="C150" s="4" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="151" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A151" s="9"/>
+      <c r="B151" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="C151" s="4" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="152" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A152" s="9"/>
+      <c r="B152" s="9" t="s">
+        <v>3</v>
+      </c>
+      <c r="C152" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="153" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A153" s="9"/>
+      <c r="B153" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="C153" s="4" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="154" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A154" s="9"/>
+      <c r="B154" s="9" t="s">
+        <v>51</v>
+      </c>
+      <c r="C154" s="14" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="155" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A155" s="9"/>
+      <c r="B155" s="12" t="s">
+        <v>52</v>
+      </c>
+      <c r="C155" s="15" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="156" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A156" s="9"/>
+      <c r="B156" s="9"/>
+      <c r="C156" s="4"/>
+    </row>
+    <row r="157" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A157" s="9" t="s">
+        <v>57</v>
+      </c>
+      <c r="B157" s="9"/>
+      <c r="C157" s="4"/>
+    </row>
+    <row r="158" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A158" s="9"/>
+      <c r="B158" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="C158" s="4" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="159" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A159" s="9"/>
+      <c r="B159" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="C159" s="4" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="160" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A160" s="9"/>
+      <c r="B160" s="9" t="s">
+        <v>3</v>
+      </c>
+      <c r="C160" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="161" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A161" s="9"/>
+      <c r="B161" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="C161" s="4" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="162" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A162" s="9"/>
+      <c r="B162" s="9" t="s">
+        <v>51</v>
+      </c>
+      <c r="C162" s="14" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="163" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A163" s="9"/>
+      <c r="B163" s="12" t="s">
+        <v>52</v>
+      </c>
+      <c r="C163" s="15" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="164" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A164" s="7"/>
+      <c r="B164" s="7"/>
+      <c r="C164" s="8"/>
+    </row>
+    <row r="165" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A165" s="9" t="s">
+        <v>71</v>
+      </c>
+      <c r="B165" s="9"/>
+      <c r="C165" s="4"/>
+    </row>
+    <row r="166" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A166" s="9"/>
+      <c r="B166" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="C166" s="4" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="167" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A167" s="9"/>
+      <c r="B167" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="C167" s="4" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="168" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A168" s="9"/>
+      <c r="B168" s="9" t="s">
+        <v>3</v>
+      </c>
+      <c r="C168" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="169" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A169" s="9"/>
+      <c r="B169" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="C169" s="4" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="170" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A170" s="9"/>
+      <c r="B170" s="9" t="s">
+        <v>51</v>
+      </c>
+      <c r="C170" s="14" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="171" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A171" s="9"/>
+      <c r="B171" s="12" t="s">
+        <v>52</v>
+      </c>
+      <c r="C171" s="15" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="172" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A172" s="9"/>
+      <c r="B172" s="9"/>
+      <c r="C172" s="4"/>
+    </row>
+    <row r="173" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A173" s="9" t="s">
+        <v>72</v>
+      </c>
+      <c r="B173" s="9"/>
+      <c r="C173" s="4"/>
+    </row>
+    <row r="174" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A174" s="9"/>
+      <c r="B174" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="C174" s="4" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="175" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A175" s="9"/>
+      <c r="B175" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="C175" s="4" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="176" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A176" s="9"/>
+      <c r="B176" s="9" t="s">
+        <v>3</v>
+      </c>
+      <c r="C176" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="177" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A177" s="9"/>
+      <c r="B177" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="C177" s="4" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="178" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A178" s="9"/>
+      <c r="B178" s="9" t="s">
+        <v>51</v>
+      </c>
+      <c r="C178" s="14" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="179" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A179" s="9"/>
+      <c r="B179" s="12" t="s">
+        <v>52</v>
+      </c>
+      <c r="C179" s="15" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="180" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A180" s="9"/>
+      <c r="B180" s="9"/>
+      <c r="C180" s="4"/>
+    </row>
+    <row r="181" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A181" s="9" t="s">
+        <v>61</v>
+      </c>
+      <c r="B181" s="9"/>
+      <c r="C181" s="4"/>
+    </row>
+    <row r="182" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A182" s="9"/>
+      <c r="B182" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="C182" s="4" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="183" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A183" s="9"/>
+      <c r="B183" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="C183" s="4" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="184" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A184" s="9"/>
+      <c r="B184" s="9" t="s">
+        <v>3</v>
+      </c>
+      <c r="C184" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="185" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A185" s="9"/>
+      <c r="B185" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="C185" s="4" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="186" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A186" s="9"/>
+      <c r="B186" s="9" t="s">
+        <v>51</v>
+      </c>
+      <c r="C186" s="14" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="187" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A187" s="9"/>
+      <c r="B187" s="12" t="s">
+        <v>52</v>
+      </c>
+      <c r="C187" s="15" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="188" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A188" s="9"/>
+      <c r="B188" s="9"/>
+      <c r="C188" s="4"/>
+    </row>
+    <row r="189" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A189" s="9" t="s">
+        <v>63</v>
+      </c>
+      <c r="B189" s="9"/>
+      <c r="C189" s="4"/>
+    </row>
+    <row r="190" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A190" s="9"/>
+      <c r="B190" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="C190" s="4" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="191" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A191" s="9"/>
+      <c r="B191" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="C191" s="4" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="192" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A192" s="9"/>
+      <c r="B192" s="9" t="s">
+        <v>3</v>
+      </c>
+      <c r="C192" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="193" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A193" s="9"/>
+      <c r="B193" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="C193" s="4" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="194" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A194" s="9"/>
+      <c r="B194" s="9" t="s">
+        <v>51</v>
+      </c>
+      <c r="C194" s="14" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="195" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A195" s="9"/>
+      <c r="B195" s="12" t="s">
+        <v>52</v>
+      </c>
+      <c r="C195" s="15" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="196" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A196" s="9"/>
+      <c r="B196" s="9"/>
+      <c r="C196" s="4"/>
+    </row>
+    <row r="197" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A197" s="9" t="s">
+        <v>65</v>
+      </c>
+      <c r="B197" s="9"/>
+      <c r="C197" s="4"/>
+    </row>
+    <row r="198" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A198" s="9"/>
+      <c r="B198" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="C198" s="4" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="199" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A199" s="9"/>
+      <c r="B199" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="C199" s="4" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="200" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A200" s="9"/>
+      <c r="B200" s="9" t="s">
+        <v>3</v>
+      </c>
+      <c r="C200" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="201" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A201" s="9"/>
+      <c r="B201" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="C201" s="4" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="202" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A202" s="9"/>
+      <c r="B202" s="9" t="s">
+        <v>51</v>
+      </c>
+      <c r="C202" s="14" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="139" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A139" s="11"/>
-      <c r="B139" s="15" t="s">
-        <v>53</v>
-      </c>
-      <c r="C139" s="18" t="s">
+    <row r="203" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A203" s="9"/>
+      <c r="B203" s="12" t="s">
+        <v>52</v>
+      </c>
+      <c r="C203" s="15" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="140" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A140" s="11"/>
-      <c r="B140" s="11"/>
-      <c r="C140" s="5"/>
-    </row>
-    <row r="141" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A141" s="11" t="s">
-        <v>54</v>
-      </c>
-      <c r="B141" s="11"/>
-      <c r="C141" s="5"/>
-    </row>
-    <row r="142" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A142" s="11"/>
-      <c r="B142" s="11" t="s">
+    <row r="204" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A204" s="9"/>
+      <c r="B204" s="9"/>
+      <c r="C204" s="4"/>
+    </row>
+    <row r="205" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A205" s="9" t="s">
+        <v>67</v>
+      </c>
+      <c r="B205" s="9"/>
+      <c r="C205" s="4"/>
+    </row>
+    <row r="206" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A206" s="9"/>
+      <c r="B206" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="C142" s="5" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="143" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A143" s="11"/>
-      <c r="B143" s="11" t="s">
+      <c r="C206" s="4" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="207" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A207" s="9"/>
+      <c r="B207" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="C143" s="5" t="s">
+      <c r="C207" s="4" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="144" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A144" s="11"/>
-      <c r="B144" s="11" t="s">
+    <row r="208" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A208" s="9"/>
+      <c r="B208" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="C144" s="7">
+      <c r="C208" s="6">
         <v>1</v>
       </c>
     </row>
-    <row r="145" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A145" s="11"/>
-      <c r="B145" s="11" t="s">
+    <row r="209" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A209" s="9"/>
+      <c r="B209" s="9" t="s">
         <v>14</v>
       </c>
-      <c r="C145" s="5" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="146" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A146" s="11"/>
-      <c r="B146" s="11" t="s">
+      <c r="C209" s="4" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="210" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A210" s="9"/>
+      <c r="B210" s="9" t="s">
+        <v>51</v>
+      </c>
+      <c r="C210" s="14" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="211" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A211" s="9"/>
+      <c r="B211" s="12" t="s">
         <v>52</v>
       </c>
-      <c r="C146" s="17" t="s">
+      <c r="C211" s="15" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="212" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A212" s="9"/>
+      <c r="B212" s="9"/>
+      <c r="C212" s="4"/>
+    </row>
+    <row r="213" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A213" s="9" t="s">
+        <v>69</v>
+      </c>
+      <c r="B213" s="9"/>
+      <c r="C213" s="4"/>
+    </row>
+    <row r="214" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A214" s="9"/>
+      <c r="B214" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="C214" s="4" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="215" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A215" s="9"/>
+      <c r="B215" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="C215" s="4" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="216" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A216" s="9"/>
+      <c r="B216" s="9" t="s">
+        <v>3</v>
+      </c>
+      <c r="C216" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="217" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A217" s="9"/>
+      <c r="B217" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="C217" s="4" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="218" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A218" s="9"/>
+      <c r="B218" s="9" t="s">
+        <v>51</v>
+      </c>
+      <c r="C218" s="14" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="147" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A147" s="11"/>
-      <c r="B147" s="15" t="s">
-        <v>53</v>
-      </c>
-      <c r="C147" s="18" t="s">
+    <row r="219" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A219" s="9"/>
+      <c r="B219" s="12" t="s">
+        <v>52</v>
+      </c>
+      <c r="C219" s="15" t="s">
         <v>81</v>
-      </c>
-    </row>
-    <row r="148" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A148" s="11"/>
-      <c r="B148" s="11"/>
-      <c r="C148" s="5"/>
-    </row>
-    <row r="149" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A149" s="11" t="s">
-        <v>56</v>
-      </c>
-      <c r="B149" s="11"/>
-      <c r="C149" s="5"/>
-    </row>
-    <row r="150" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A150" s="11"/>
-      <c r="B150" s="11" t="s">
-        <v>8</v>
-      </c>
-      <c r="C150" s="5" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="151" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A151" s="11"/>
-      <c r="B151" s="11" t="s">
-        <v>10</v>
-      </c>
-      <c r="C151" s="5" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="152" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A152" s="11"/>
-      <c r="B152" s="11" t="s">
-        <v>3</v>
-      </c>
-      <c r="C152" s="7">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="153" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A153" s="11"/>
-      <c r="B153" s="11" t="s">
-        <v>14</v>
-      </c>
-      <c r="C153" s="5" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="154" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A154" s="11"/>
-      <c r="B154" s="11" t="s">
-        <v>52</v>
-      </c>
-      <c r="C154" s="17" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="155" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A155" s="11"/>
-      <c r="B155" s="15" t="s">
-        <v>53</v>
-      </c>
-      <c r="C155" s="18" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="156" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A156" s="11"/>
-      <c r="B156" s="11"/>
-      <c r="C156" s="5"/>
-    </row>
-    <row r="157" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A157" s="11" t="s">
-        <v>58</v>
-      </c>
-      <c r="B157" s="11"/>
-      <c r="C157" s="5"/>
-    </row>
-    <row r="158" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A158" s="11"/>
-      <c r="B158" s="11" t="s">
-        <v>8</v>
-      </c>
-      <c r="C158" s="5" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="159" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A159" s="11"/>
-      <c r="B159" s="11" t="s">
-        <v>10</v>
-      </c>
-      <c r="C159" s="5" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="160" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A160" s="11"/>
-      <c r="B160" s="11" t="s">
-        <v>3</v>
-      </c>
-      <c r="C160" s="7">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="161" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A161" s="11"/>
-      <c r="B161" s="11" t="s">
-        <v>14</v>
-      </c>
-      <c r="C161" s="5" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="162" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A162" s="11"/>
-      <c r="B162" s="11" t="s">
-        <v>52</v>
-      </c>
-      <c r="C162" s="17" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="163" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A163" s="11"/>
-      <c r="B163" s="15" t="s">
-        <v>53</v>
-      </c>
-      <c r="C163" s="18" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="164" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A164" s="8"/>
-      <c r="B164" s="8"/>
-      <c r="C164" s="9"/>
-    </row>
-    <row r="165" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A165" s="11" t="s">
-        <v>72</v>
-      </c>
-      <c r="B165" s="11"/>
-      <c r="C165" s="5"/>
-    </row>
-    <row r="166" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A166" s="11"/>
-      <c r="B166" s="11" t="s">
-        <v>8</v>
-      </c>
-      <c r="C166" s="5" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="167" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A167" s="11"/>
-      <c r="B167" s="11" t="s">
-        <v>10</v>
-      </c>
-      <c r="C167" s="5" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="168" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A168" s="11"/>
-      <c r="B168" s="11" t="s">
-        <v>3</v>
-      </c>
-      <c r="C168" s="7">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="169" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A169" s="11"/>
-      <c r="B169" s="11" t="s">
-        <v>14</v>
-      </c>
-      <c r="C169" s="5" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="170" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A170" s="11"/>
-      <c r="B170" s="11" t="s">
-        <v>52</v>
-      </c>
-      <c r="C170" s="17" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="171" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A171" s="11"/>
-      <c r="B171" s="15" t="s">
-        <v>53</v>
-      </c>
-      <c r="C171" s="18" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="172" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A172" s="11"/>
-      <c r="B172" s="11"/>
-      <c r="C172" s="5"/>
-    </row>
-    <row r="173" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A173" s="11" t="s">
-        <v>73</v>
-      </c>
-      <c r="B173" s="11"/>
-      <c r="C173" s="5"/>
-    </row>
-    <row r="174" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A174" s="11"/>
-      <c r="B174" s="11" t="s">
-        <v>8</v>
-      </c>
-      <c r="C174" s="5" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="175" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A175" s="11"/>
-      <c r="B175" s="11" t="s">
-        <v>10</v>
-      </c>
-      <c r="C175" s="5" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="176" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A176" s="11"/>
-      <c r="B176" s="11" t="s">
-        <v>3</v>
-      </c>
-      <c r="C176" s="7">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="177" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A177" s="11"/>
-      <c r="B177" s="11" t="s">
-        <v>14</v>
-      </c>
-      <c r="C177" s="5" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="178" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A178" s="11"/>
-      <c r="B178" s="11" t="s">
-        <v>52</v>
-      </c>
-      <c r="C178" s="17" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="179" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A179" s="11"/>
-      <c r="B179" s="15" t="s">
-        <v>53</v>
-      </c>
-      <c r="C179" s="18" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="180" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A180" s="11"/>
-      <c r="B180" s="11"/>
-      <c r="C180" s="5"/>
-    </row>
-    <row r="181" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A181" s="11" t="s">
-        <v>62</v>
-      </c>
-      <c r="B181" s="11"/>
-      <c r="C181" s="5"/>
-    </row>
-    <row r="182" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A182" s="11"/>
-      <c r="B182" s="11" t="s">
-        <v>8</v>
-      </c>
-      <c r="C182" s="5" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="183" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A183" s="11"/>
-      <c r="B183" s="11" t="s">
-        <v>10</v>
-      </c>
-      <c r="C183" s="5" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="184" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A184" s="11"/>
-      <c r="B184" s="11" t="s">
-        <v>3</v>
-      </c>
-      <c r="C184" s="7">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="185" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A185" s="11"/>
-      <c r="B185" s="11" t="s">
-        <v>14</v>
-      </c>
-      <c r="C185" s="5" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="186" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A186" s="11"/>
-      <c r="B186" s="11" t="s">
-        <v>52</v>
-      </c>
-      <c r="C186" s="17" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="187" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A187" s="11"/>
-      <c r="B187" s="15" t="s">
-        <v>53</v>
-      </c>
-      <c r="C187" s="18" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="188" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A188" s="11"/>
-      <c r="B188" s="11"/>
-      <c r="C188" s="5"/>
-    </row>
-    <row r="189" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A189" s="11" t="s">
-        <v>64</v>
-      </c>
-      <c r="B189" s="11"/>
-      <c r="C189" s="5"/>
-    </row>
-    <row r="190" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A190" s="11"/>
-      <c r="B190" s="11" t="s">
-        <v>8</v>
-      </c>
-      <c r="C190" s="5" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="191" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A191" s="11"/>
-      <c r="B191" s="11" t="s">
-        <v>10</v>
-      </c>
-      <c r="C191" s="5" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="192" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A192" s="11"/>
-      <c r="B192" s="11" t="s">
-        <v>3</v>
-      </c>
-      <c r="C192" s="7">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="193" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A193" s="11"/>
-      <c r="B193" s="11" t="s">
-        <v>14</v>
-      </c>
-      <c r="C193" s="5" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="194" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A194" s="11"/>
-      <c r="B194" s="11" t="s">
-        <v>52</v>
-      </c>
-      <c r="C194" s="17" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="195" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A195" s="11"/>
-      <c r="B195" s="15" t="s">
-        <v>53</v>
-      </c>
-      <c r="C195" s="18" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="196" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A196" s="11"/>
-      <c r="B196" s="11"/>
-      <c r="C196" s="5"/>
-    </row>
-    <row r="197" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A197" s="11" t="s">
-        <v>66</v>
-      </c>
-      <c r="B197" s="11"/>
-      <c r="C197" s="5"/>
-    </row>
-    <row r="198" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A198" s="11"/>
-      <c r="B198" s="11" t="s">
-        <v>8</v>
-      </c>
-      <c r="C198" s="5" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="199" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A199" s="11"/>
-      <c r="B199" s="11" t="s">
-        <v>10</v>
-      </c>
-      <c r="C199" s="5" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="200" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A200" s="11"/>
-      <c r="B200" s="11" t="s">
-        <v>3</v>
-      </c>
-      <c r="C200" s="7">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="201" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A201" s="11"/>
-      <c r="B201" s="11" t="s">
-        <v>14</v>
-      </c>
-      <c r="C201" s="5" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="202" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A202" s="11"/>
-      <c r="B202" s="11" t="s">
-        <v>52</v>
-      </c>
-      <c r="C202" s="17" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="203" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A203" s="11"/>
-      <c r="B203" s="15" t="s">
-        <v>53</v>
-      </c>
-      <c r="C203" s="18" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="204" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A204" s="11"/>
-      <c r="B204" s="11"/>
-      <c r="C204" s="5"/>
-    </row>
-    <row r="205" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A205" s="11" t="s">
-        <v>68</v>
-      </c>
-      <c r="B205" s="11"/>
-      <c r="C205" s="5"/>
-    </row>
-    <row r="206" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A206" s="11"/>
-      <c r="B206" s="11" t="s">
-        <v>8</v>
-      </c>
-      <c r="C206" s="5" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="207" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A207" s="11"/>
-      <c r="B207" s="11" t="s">
-        <v>10</v>
-      </c>
-      <c r="C207" s="5" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="208" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A208" s="11"/>
-      <c r="B208" s="11" t="s">
-        <v>3</v>
-      </c>
-      <c r="C208" s="7">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="209" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A209" s="11"/>
-      <c r="B209" s="11" t="s">
-        <v>14</v>
-      </c>
-      <c r="C209" s="5" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="210" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A210" s="11"/>
-      <c r="B210" s="11" t="s">
-        <v>52</v>
-      </c>
-      <c r="C210" s="17" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="211" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A211" s="11"/>
-      <c r="B211" s="15" t="s">
-        <v>53</v>
-      </c>
-      <c r="C211" s="18" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="212" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A212" s="11"/>
-      <c r="B212" s="11"/>
-      <c r="C212" s="5"/>
-    </row>
-    <row r="213" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A213" s="11" t="s">
-        <v>70</v>
-      </c>
-      <c r="B213" s="11"/>
-      <c r="C213" s="5"/>
-    </row>
-    <row r="214" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A214" s="11"/>
-      <c r="B214" s="11" t="s">
-        <v>8</v>
-      </c>
-      <c r="C214" s="5" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="215" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A215" s="11"/>
-      <c r="B215" s="11" t="s">
-        <v>10</v>
-      </c>
-      <c r="C215" s="5" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="216" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A216" s="11"/>
-      <c r="B216" s="11" t="s">
-        <v>3</v>
-      </c>
-      <c r="C216" s="7">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="217" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A217" s="11"/>
-      <c r="B217" s="11" t="s">
-        <v>14</v>
-      </c>
-      <c r="C217" s="5" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="218" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A218" s="11"/>
-      <c r="B218" s="11" t="s">
-        <v>52</v>
-      </c>
-      <c r="C218" s="17" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="219" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A219" s="11"/>
-      <c r="B219" s="15" t="s">
-        <v>53</v>
-      </c>
-      <c r="C219" s="18" t="s">
-        <v>83</v>
       </c>
     </row>
     <row r="220" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">

</xml_diff>